<commit_message>
Improved logging and data caching. Using Adam optimizer now.
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -482,6 +482,381 @@
         <v>465.7879297330433</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>-x**2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.08142967522144318</v>
+      </c>
+      <c r="F3" t="n">
+        <v>19.83478403091431</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1008.329607664404</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>x**2</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2.086819613799132e-15</v>
+      </c>
+      <c r="F4" t="n">
+        <v>16.9700231552124</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1178.548774923559</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>-x**2</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.00125144375488162</v>
+      </c>
+      <c r="F5" t="n">
+        <v>16.89823484420776</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1183.555571596014</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.000135384892928414</v>
+      </c>
+      <c r="F6" t="n">
+        <v>79.72848176956177</v>
+      </c>
+      <c r="G6" t="n">
+        <v>250.8513840487487</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>-x**2</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.16468106625689e-06</v>
+      </c>
+      <c r="F7" t="n">
+        <v>23.01174783706665</v>
+      </c>
+      <c r="G7" t="n">
+        <v>869.1212915076613</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sin(5*x)</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0003030607185792178</v>
+      </c>
+      <c r="F8" t="n">
+        <v>49.36098575592041</v>
+      </c>
+      <c r="G8" t="n">
+        <v>405.178294025483</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.000135384892928414</v>
+      </c>
+      <c r="F9" t="n">
+        <v>80.61733603477478</v>
+      </c>
+      <c r="G9" t="n">
+        <v>248.0855977599269</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0002126327308360487</v>
+      </c>
+      <c r="F10" t="n">
+        <v>83.81179332733154</v>
+      </c>
+      <c r="G10" t="n">
+        <v>238.6299016641835</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0002079298283206299</v>
+      </c>
+      <c r="F11" t="n">
+        <v>83.99549984931946</v>
+      </c>
+      <c r="G11" t="n">
+        <v>238.1079943077694</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0002149988722521812</v>
+      </c>
+      <c r="F12" t="n">
+        <v>82.73853874206543</v>
+      </c>
+      <c r="G12" t="n">
+        <v>241.7253229761444</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.0002149988722521812</v>
+      </c>
+      <c r="F13" t="n">
+        <v>82.53280305862427</v>
+      </c>
+      <c r="G13" t="n">
+        <v>242.3278897457742</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>4</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0002149988722521812</v>
+      </c>
+      <c r="F14" t="n">
+        <v>83.14774823188782</v>
+      </c>
+      <c r="G14" t="n">
+        <v>240.5356780585652</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.0002149988722521812</v>
+      </c>
+      <c r="F15" t="n">
+        <v>82.21243619918823</v>
+      </c>
+      <c r="G15" t="n">
+        <v>243.2721973053206</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0002149988722521812</v>
+      </c>
+      <c r="F16" t="n">
+        <v>82.92414236068726</v>
+      </c>
+      <c r="G16" t="n">
+        <v>241.184285186911</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C17" t="n">
+        <v>4</v>
+      </c>
+      <c r="D17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0002149988722521812</v>
+      </c>
+      <c r="F17" t="n">
+        <v>80.24481797218323</v>
+      </c>
+      <c r="G17" t="n">
+        <v>249.2372779377851</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Option to rerun old experiments from logged data
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -857,6 +857,31 @@
         <v>249.2372779377851</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>x**2</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0004686458851210773</v>
+      </c>
+      <c r="F18" t="n">
+        <v>22.45450019836426</v>
+      </c>
+      <c r="G18" t="n">
+        <v>890.6900542572281</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added script for batch performance testing and evaluation.
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -456,6 +456,12 @@
           <t>Iters per Second</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Success</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,6 +487,8 @@
       <c r="G2" t="n">
         <v>465.7879297330433</v>
       </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -506,6 +514,8 @@
       <c r="G3" t="n">
         <v>1008.329607664404</v>
       </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -531,6 +541,8 @@
       <c r="G4" t="n">
         <v>1178.548774923559</v>
       </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -556,6 +568,8 @@
       <c r="G5" t="n">
         <v>1183.555571596014</v>
       </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -581,6 +595,8 @@
       <c r="G6" t="n">
         <v>250.8513840487487</v>
       </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -606,6 +622,8 @@
       <c r="G7" t="n">
         <v>869.1212915076613</v>
       </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -631,6 +649,8 @@
       <c r="G8" t="n">
         <v>405.178294025483</v>
       </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -656,6 +676,8 @@
       <c r="G9" t="n">
         <v>248.0855977599269</v>
       </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -681,6 +703,8 @@
       <c r="G10" t="n">
         <v>238.6299016641835</v>
       </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -706,6 +730,8 @@
       <c r="G11" t="n">
         <v>238.1079943077694</v>
       </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -731,6 +757,8 @@
       <c r="G12" t="n">
         <v>241.7253229761444</v>
       </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -756,6 +784,8 @@
       <c r="G13" t="n">
         <v>242.3278897457742</v>
       </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -781,6 +811,8 @@
       <c r="G14" t="n">
         <v>240.5356780585652</v>
       </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -806,6 +838,8 @@
       <c r="G15" t="n">
         <v>243.2721973053206</v>
       </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -831,6 +865,8 @@
       <c r="G16" t="n">
         <v>241.184285186911</v>
       </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -856,6 +892,8 @@
       <c r="G17" t="n">
         <v>249.2372779377851</v>
       </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -880,6 +918,1796 @@
       </c>
       <c r="G18" t="n">
         <v>890.6900542572281</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>5*x**5 + 5*x**4 - 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.1978529393672943</v>
+      </c>
+      <c r="F19" t="n">
+        <v>22.39950442314148</v>
+      </c>
+      <c r="G19" t="n">
+        <v>892.8768968360527</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>5*x**5 + 5*x**4 - 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.0003000034193973988</v>
+      </c>
+      <c r="F20" t="n">
+        <v>46.22021126747131</v>
+      </c>
+      <c r="G20" t="n">
+        <v>432.7111333235191</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.4623310267925262</v>
+      </c>
+      <c r="F21" t="n">
+        <v>82.70141959190369</v>
+      </c>
+      <c r="G21" t="n">
+        <v>241.8338173478943</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F22" t="n">
+        <v>81.45092940330505</v>
+      </c>
+      <c r="G22" t="n">
+        <v>245.5466149559793</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F23" t="n">
+        <v>86.48769760131836</v>
+      </c>
+      <c r="G23" t="n">
+        <v>231.2467617324471</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" t="n">
+        <v>4</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F24" t="n">
+        <v>84.83793711662292</v>
+      </c>
+      <c r="G24" t="n">
+        <v>235.7435916022674</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" t="n">
+        <v>4</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F25" t="n">
+        <v>81.71687293052673</v>
+      </c>
+      <c r="G25" t="n">
+        <v>244.7474956243542</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" t="n">
+        <v>4</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F26" t="n">
+        <v>82.11606907844543</v>
+      </c>
+      <c r="G26" t="n">
+        <v>243.5576888232924</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F27" t="n">
+        <v>82.0576331615448</v>
+      </c>
+      <c r="G27" t="n">
+        <v>243.7311341971868</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F28" t="n">
+        <v>84.2228832244873</v>
+      </c>
+      <c r="G28" t="n">
+        <v>237.4651547690678</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C29" t="n">
+        <v>4</v>
+      </c>
+      <c r="D29" t="n">
+        <v>4</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F29" t="n">
+        <v>81.96315884590149</v>
+      </c>
+      <c r="G29" t="n">
+        <v>244.0120693444953</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" t="n">
+        <v>4</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F30" t="n">
+        <v>83.0768461227417</v>
+      </c>
+      <c r="G30" t="n">
+        <v>240.7409637391752</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F31" t="n">
+        <v>80.10435628890991</v>
+      </c>
+      <c r="G31" t="n">
+        <v>249.6743114427712</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F32" t="n">
+        <v>80.48693823814392</v>
+      </c>
+      <c r="G32" t="n">
+        <v>248.4875240355672</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F33" t="n">
+        <v>82.16846561431885</v>
+      </c>
+      <c r="G33" t="n">
+        <v>243.4023788867582</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F34" t="n">
+        <v>82.15730595588684</v>
+      </c>
+      <c r="G34" t="n">
+        <v>243.4354409179228</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F35" t="n">
+        <v>82.31668424606323</v>
+      </c>
+      <c r="G35" t="n">
+        <v>242.9641108990186</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4</v>
+      </c>
+      <c r="D36" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F36" t="n">
+        <v>81.74866151809692</v>
+      </c>
+      <c r="G36" t="n">
+        <v>244.652323702848</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C37" t="n">
+        <v>4</v>
+      </c>
+      <c r="D37" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F37" t="n">
+        <v>80.96949553489685</v>
+      </c>
+      <c r="G37" t="n">
+        <v>247.0066025220603</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C38" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" t="n">
+        <v>4</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F38" t="n">
+        <v>81.21751856803894</v>
+      </c>
+      <c r="G38" t="n">
+        <v>246.2522907941992</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C39" t="n">
+        <v>4</v>
+      </c>
+      <c r="D39" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F39" t="n">
+        <v>81.50102829933167</v>
+      </c>
+      <c r="G39" t="n">
+        <v>245.3956768072337</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C40" t="n">
+        <v>4</v>
+      </c>
+      <c r="D40" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F40" t="n">
+        <v>81.36474251747131</v>
+      </c>
+      <c r="G40" t="n">
+        <v>245.8067140777276</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C41" t="n">
+        <v>4</v>
+      </c>
+      <c r="D41" t="n">
+        <v>4</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F41" t="n">
+        <v>81.06601738929749</v>
+      </c>
+      <c r="G41" t="n">
+        <v>246.7125022801533</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C42" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" t="n">
+        <v>4</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.0002302447101101279</v>
+      </c>
+      <c r="F42" t="n">
+        <v>80.80536222457886</v>
+      </c>
+      <c r="G42" t="n">
+        <v>247.5083267916659</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>sin(20*x)</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>200</v>
+      </c>
+      <c r="C43" t="n">
+        <v>4</v>
+      </c>
+      <c r="D43" t="n">
+        <v>4</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.4408266544342041</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2.308500051498413</v>
+      </c>
+      <c r="G43" t="n">
+        <v>86.63634201358713</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>sin(20*x)</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C44" t="n">
+        <v>7</v>
+      </c>
+      <c r="D44" t="n">
+        <v>7</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.3708386123180389</v>
+      </c>
+      <c r="F44" t="n">
+        <v>14.31501412391663</v>
+      </c>
+      <c r="G44" t="n">
+        <v>139.7134492978617</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C45" t="n">
+        <v>4</v>
+      </c>
+      <c r="D45" t="n">
+        <v>4</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.0007102209492586553</v>
+      </c>
+      <c r="F45" t="n">
+        <v>76.22889256477356</v>
+      </c>
+      <c r="G45" t="n">
+        <v>262.3677102878742</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C46" t="n">
+        <v>4</v>
+      </c>
+      <c r="D46" t="n">
+        <v>4</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.009363508783280849</v>
+      </c>
+      <c r="F46" t="n">
+        <v>82.01628971099854</v>
+      </c>
+      <c r="G46" t="n">
+        <v>243.8539962058045</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C47" t="n">
+        <v>4</v>
+      </c>
+      <c r="D47" t="n">
+        <v>4</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.000133225490571931</v>
+      </c>
+      <c r="F47" t="n">
+        <v>81.13004064559937</v>
+      </c>
+      <c r="G47" t="n">
+        <v>246.5178106759008</v>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C48" t="n">
+        <v>4</v>
+      </c>
+      <c r="D48" t="n">
+        <v>4</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.0001406475494150072</v>
+      </c>
+      <c r="F48" t="n">
+        <v>81.53274703025818</v>
+      </c>
+      <c r="G48" t="n">
+        <v>245.3002103875841</v>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C49" t="n">
+        <v>4</v>
+      </c>
+      <c r="D49" t="n">
+        <v>4</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.0007071758154779673</v>
+      </c>
+      <c r="F49" t="n">
+        <v>80.84686064720154</v>
+      </c>
+      <c r="G49" t="n">
+        <v>247.3812815970151</v>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C50" t="n">
+        <v>4</v>
+      </c>
+      <c r="D50" t="n">
+        <v>4</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.001180937513709068</v>
+      </c>
+      <c r="F50" t="n">
+        <v>80.93430924415588</v>
+      </c>
+      <c r="G50" t="n">
+        <v>247.1139889470813</v>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C51" t="n">
+        <v>4</v>
+      </c>
+      <c r="D51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.0001657234679441899</v>
+      </c>
+      <c r="F51" t="n">
+        <v>81.4379301071167</v>
+      </c>
+      <c r="G51" t="n">
+        <v>245.5858096306434</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C52" t="n">
+        <v>4</v>
+      </c>
+      <c r="D52" t="n">
+        <v>4</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.000126074708532542</v>
+      </c>
+      <c r="F52" t="n">
+        <v>81.47728538513184</v>
+      </c>
+      <c r="G52" t="n">
+        <v>245.467186412296</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C53" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" t="n">
+        <v>4</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.0001202542262035422</v>
+      </c>
+      <c r="F53" t="n">
+        <v>81.5821545124054</v>
+      </c>
+      <c r="G53" t="n">
+        <v>245.1516525830266</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C54" t="n">
+        <v>4</v>
+      </c>
+      <c r="D54" t="n">
+        <v>4</v>
+      </c>
+      <c r="E54" t="n">
+        <v>9.688065620139241e-05</v>
+      </c>
+      <c r="F54" t="n">
+        <v>81.64172530174255</v>
+      </c>
+      <c r="G54" t="n">
+        <v>244.9727749637981</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C55" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" t="n">
+        <v>4</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.0001163358319899999</v>
+      </c>
+      <c r="F55" t="n">
+        <v>84.28910779953003</v>
+      </c>
+      <c r="G55" t="n">
+        <v>237.2785822762204</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C56" t="n">
+        <v>4</v>
+      </c>
+      <c r="D56" t="n">
+        <v>4</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.000173839638591744</v>
+      </c>
+      <c r="F56" t="n">
+        <v>91.2928421497345</v>
+      </c>
+      <c r="G56" t="n">
+        <v>219.0752257137189</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C57" t="n">
+        <v>4</v>
+      </c>
+      <c r="D57" t="n">
+        <v>4</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.721627945196815e-05</v>
+      </c>
+      <c r="F57" t="n">
+        <v>98.25150632858276</v>
+      </c>
+      <c r="G57" t="n">
+        <v>203.5592200806973</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C58" t="n">
+        <v>4</v>
+      </c>
+      <c r="D58" t="n">
+        <v>4</v>
+      </c>
+      <c r="E58" t="n">
+        <v>7.031946006463841e-05</v>
+      </c>
+      <c r="F58" t="n">
+        <v>105.1464288234711</v>
+      </c>
+      <c r="G58" t="n">
+        <v>190.2109298792994</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C59" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" t="n">
+        <v>4</v>
+      </c>
+      <c r="E59" t="n">
+        <v>4.012827048427425e-05</v>
+      </c>
+      <c r="F59" t="n">
+        <v>112.2540347576141</v>
+      </c>
+      <c r="G59" t="n">
+        <v>178.1673152611863</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C60" t="n">
+        <v>4</v>
+      </c>
+      <c r="D60" t="n">
+        <v>4</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.0001453561999369413</v>
+      </c>
+      <c r="F60" t="n">
+        <v>118.4494695663452</v>
+      </c>
+      <c r="G60" t="n">
+        <v>168.8483711511913</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C61" t="n">
+        <v>4</v>
+      </c>
+      <c r="D61" t="n">
+        <v>4</v>
+      </c>
+      <c r="E61" t="n">
+        <v>8.815047476673499e-05</v>
+      </c>
+      <c r="F61" t="n">
+        <v>125.8994338512421</v>
+      </c>
+      <c r="G61" t="n">
+        <v>158.856949457225</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C62" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" t="n">
+        <v>4</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.0001623907737666741</v>
+      </c>
+      <c r="F62" t="n">
+        <v>132.6842293739319</v>
+      </c>
+      <c r="G62" t="n">
+        <v>150.7338143679142</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C63" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" t="n">
+        <v>4</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.0001735917467158288</v>
+      </c>
+      <c r="F63" t="n">
+        <v>141.32341837883</v>
+      </c>
+      <c r="G63" t="n">
+        <v>141.5193619672306</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C64" t="n">
+        <v>4</v>
+      </c>
+      <c r="D64" t="n">
+        <v>4</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.0001263737358385697</v>
+      </c>
+      <c r="F64" t="n">
+        <v>145.6846284866333</v>
+      </c>
+      <c r="G64" t="n">
+        <v>137.2828431369821</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C65" t="n">
+        <v>4</v>
+      </c>
+      <c r="D65" t="n">
+        <v>4</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.0002068333851639181</v>
+      </c>
+      <c r="F65" t="n">
+        <v>152.9530162811279</v>
+      </c>
+      <c r="G65" t="n">
+        <v>130.7591081645619</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C66" t="n">
+        <v>4</v>
+      </c>
+      <c r="D66" t="n">
+        <v>4</v>
+      </c>
+      <c r="E66" t="n">
+        <v>9.939885785570368e-05</v>
+      </c>
+      <c r="F66" t="n">
+        <v>161.2642805576324</v>
+      </c>
+      <c r="G66" t="n">
+        <v>124.0200243404331</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C67" t="n">
+        <v>4</v>
+      </c>
+      <c r="D67" t="n">
+        <v>4</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.0001925082324305549</v>
+      </c>
+      <c r="F67" t="n">
+        <v>166.8468961715698</v>
+      </c>
+      <c r="G67" t="n">
+        <v>119.8703749300428</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C68" t="n">
+        <v>4</v>
+      </c>
+      <c r="D68" t="n">
+        <v>4</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.0001718583516776562</v>
+      </c>
+      <c r="F68" t="n">
+        <v>172.8471047878265</v>
+      </c>
+      <c r="G68" t="n">
+        <v>115.7091987427294</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C69" t="n">
+        <v>4</v>
+      </c>
+      <c r="D69" t="n">
+        <v>4</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.0001538722281111404</v>
+      </c>
+      <c r="F69" t="n">
+        <v>184.0340173244476</v>
+      </c>
+      <c r="G69" t="n">
+        <v>108.6755605880215</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C70" t="n">
+        <v>4</v>
+      </c>
+      <c r="D70" t="n">
+        <v>4</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.0001362098264507949</v>
+      </c>
+      <c r="F70" t="n">
+        <v>186.4023888111115</v>
+      </c>
+      <c r="G70" t="n">
+        <v>107.2947623019293</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Batching. Other improvements
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -458,10 +458,14 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Success</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr"/>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Autosave</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2707,6 +2711,566 @@
       <c r="I70" t="inlineStr">
         <is>
           <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C71" t="n">
+        <v>4</v>
+      </c>
+      <c r="D71" t="n">
+        <v>4</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.0007102209492586553</v>
+      </c>
+      <c r="F71" t="n">
+        <v>81.3016402721405</v>
+      </c>
+      <c r="G71" t="n">
+        <v>245.9974968900273</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C72" t="n">
+        <v>4</v>
+      </c>
+      <c r="D72" t="n">
+        <v>4</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.0007102209492586553</v>
+      </c>
+      <c r="F72" t="n">
+        <v>77.89687538146973</v>
+      </c>
+      <c r="G72" t="n">
+        <v>256.749707893388</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C73" t="n">
+        <v>4</v>
+      </c>
+      <c r="D73" t="n">
+        <v>4</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.0007102209492586553</v>
+      </c>
+      <c r="F73" t="n">
+        <v>82.5798716545105</v>
+      </c>
+      <c r="G73" t="n">
+        <v>242.1897685149478</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>25*x**5 - 50*x**4 + 100*x**3 - 200*x**2 + 400*x - 800</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C74" t="n">
+        <v>4</v>
+      </c>
+      <c r="D74" t="n">
+        <v>4</v>
+      </c>
+      <c r="E74" t="n">
+        <v>22.01958465576172</v>
+      </c>
+      <c r="F74" t="n">
+        <v>74.77325892448425</v>
+      </c>
+      <c r="G74" t="n">
+        <v>267.4753018348257</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C75" t="n">
+        <v>4</v>
+      </c>
+      <c r="D75" t="n">
+        <v>4</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.4573033154010773</v>
+      </c>
+      <c r="F75" t="n">
+        <v>77.77278709411621</v>
+      </c>
+      <c r="G75" t="n">
+        <v>257.1593580129401</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C76" t="n">
+        <v>4</v>
+      </c>
+      <c r="D76" t="n">
+        <v>4</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.04460600018501282</v>
+      </c>
+      <c r="F76" t="n">
+        <v>74.65597915649414</v>
+      </c>
+      <c r="G76" t="n">
+        <v>267.8954884253266</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C77" t="n">
+        <v>4</v>
+      </c>
+      <c r="D77" t="n">
+        <v>4</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.04698513075709343</v>
+      </c>
+      <c r="F77" t="n">
+        <v>19.63630437850952</v>
+      </c>
+      <c r="G77" t="n">
+        <v>254.630398043337</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C78" t="n">
+        <v>4</v>
+      </c>
+      <c r="D78" t="n">
+        <v>4</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.04698513075709343</v>
+      </c>
+      <c r="F78" t="n">
+        <v>20.19875931739807</v>
+      </c>
+      <c r="G78" t="n">
+        <v>247.5399563622347</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>5*x**5 - 5*x**4 + 5*x**3 - 5*x**2 + 5*x - 5</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C79" t="n">
+        <v>4</v>
+      </c>
+      <c r="D79" t="n">
+        <v>4</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.04698513075709343</v>
+      </c>
+      <c r="F79" t="n">
+        <v>20.41918420791626</v>
+      </c>
+      <c r="G79" t="n">
+        <v>244.8677649943313</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.0001324334734817967</v>
+      </c>
+      <c r="F80" t="n">
+        <v>8.728749513626099</v>
+      </c>
+      <c r="G80" t="n">
+        <v>572.8197369158895</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>tan(10*x)</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C81" t="n">
+        <v>1</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" t="n">
+        <v>3846.375244140625</v>
+      </c>
+      <c r="F81" t="n">
+        <v>8.680053234100342</v>
+      </c>
+      <c r="G81" t="n">
+        <v>576.0333335695531</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>tan(x)</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1</v>
+      </c>
+      <c r="D82" t="n">
+        <v>1</v>
+      </c>
+      <c r="E82" t="n">
+        <v>1.114379301725421e-05</v>
+      </c>
+      <c r="F82" t="n">
+        <v>8.594872951507568</v>
+      </c>
+      <c r="G82" t="n">
+        <v>581.7421651500949</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>tan(1.57*x)</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1</v>
+      </c>
+      <c r="D83" t="n">
+        <v>1</v>
+      </c>
+      <c r="E83" t="n">
+        <v>3147.503173828125</v>
+      </c>
+      <c r="F83" t="n">
+        <v>8.639046907424927</v>
+      </c>
+      <c r="G83" t="n">
+        <v>578.7675485015243</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>tan(1.57*x)</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C84" t="n">
+        <v>4</v>
+      </c>
+      <c r="D84" t="n">
+        <v>4</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2884.274169921875</v>
+      </c>
+      <c r="F84" t="n">
+        <v>20.30728888511658</v>
+      </c>
+      <c r="G84" t="n">
+        <v>246.2170124375663</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C85" t="n">
+        <v>1</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.0001320796355219922</v>
+      </c>
+      <c r="F85" t="n">
+        <v>17.51730537414551</v>
+      </c>
+      <c r="G85" t="n">
+        <v>285.4320281120234</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>sin(10*x)</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C86" t="n">
+        <v>1</v>
+      </c>
+      <c r="D86" t="n">
+        <v>1</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.0001320943410973996</v>
+      </c>
+      <c r="F86" t="n">
+        <v>18.81007742881775</v>
+      </c>
+      <c r="G86" t="n">
+        <v>265.8149610984488</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>False</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
SDF branch initial commit.
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -3309,6 +3309,41 @@
         </is>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1</v>
+      </c>
+      <c r="D88" t="n">
+        <v>1</v>
+      </c>
+      <c r="E88" t="n">
+        <v>1.008981780614704e-05</v>
+      </c>
+      <c r="F88" t="n">
+        <v>28.36333250999451</v>
+      </c>
+      <c r="G88" t="n">
+        <v>705.1357590985656</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added generators. Extended misc.
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -3344,6 +3344,1721 @@
         </is>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C89" t="n">
+        <v>1</v>
+      </c>
+      <c r="D89" t="n">
+        <v>1</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.0003267737338319421</v>
+      </c>
+      <c r="F89" t="n">
+        <v>5.825217247009277</v>
+      </c>
+      <c r="G89" t="n">
+        <v>858.3370864952802</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C90" t="n">
+        <v>1</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1</v>
+      </c>
+      <c r="E90" t="n">
+        <v>8.779316704021767e-05</v>
+      </c>
+      <c r="F90" t="n">
+        <v>6.637300252914429</v>
+      </c>
+      <c r="G90" t="n">
+        <v>753.3183387032261</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1</v>
+      </c>
+      <c r="E91" t="n">
+        <v>3.121776837033963e-09</v>
+      </c>
+      <c r="F91" t="n">
+        <v>5.173415660858154</v>
+      </c>
+      <c r="G91" t="n">
+        <v>966.4794649751015</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C92" t="n">
+        <v>1</v>
+      </c>
+      <c r="D92" t="n">
+        <v>1</v>
+      </c>
+      <c r="E92" t="n">
+        <v>1.411258381267544e-07</v>
+      </c>
+      <c r="F92" t="n">
+        <v>6.707051753997803</v>
+      </c>
+      <c r="G92" t="n">
+        <v>745.4840343254698</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C93" t="n">
+        <v>1</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1</v>
+      </c>
+      <c r="E93" t="n">
+        <v>1.28481979118078e-05</v>
+      </c>
+      <c r="F93" t="n">
+        <v>6.884666204452515</v>
+      </c>
+      <c r="G93" t="n">
+        <v>726.2516223032504</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1</v>
+      </c>
+      <c r="E94" t="n">
+        <v>1.256542054761667e-05</v>
+      </c>
+      <c r="F94" t="n">
+        <v>5.077513933181763</v>
+      </c>
+      <c r="G94" t="n">
+        <v>984.7338807530973</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C95" t="n">
+        <v>1</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.0002274225262226537</v>
+      </c>
+      <c r="F95" t="n">
+        <v>5.301516056060791</v>
+      </c>
+      <c r="G95" t="n">
+        <v>943.1264466857377</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C96" t="n">
+        <v>1</v>
+      </c>
+      <c r="D96" t="n">
+        <v>1</v>
+      </c>
+      <c r="E96" t="n">
+        <v>1.869528932729736e-05</v>
+      </c>
+      <c r="F96" t="n">
+        <v>5.28364372253418</v>
+      </c>
+      <c r="G96" t="n">
+        <v>946.3166448327185</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C97" t="n">
+        <v>1</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1</v>
+      </c>
+      <c r="E97" t="n">
+        <v>1.013629844237585e-05</v>
+      </c>
+      <c r="F97" t="n">
+        <v>7.027191400527954</v>
+      </c>
+      <c r="G97" t="n">
+        <v>711.521817895034</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C98" t="n">
+        <v>1</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2.257012738482445e-06</v>
+      </c>
+      <c r="F98" t="n">
+        <v>6.437158584594727</v>
+      </c>
+      <c r="G98" t="n">
+        <v>776.7402238568264</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C99" t="n">
+        <v>1</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1</v>
+      </c>
+      <c r="E99" t="n">
+        <v>1.504874944657786e-06</v>
+      </c>
+      <c r="F99" t="n">
+        <v>6.366659164428711</v>
+      </c>
+      <c r="G99" t="n">
+        <v>785.3412395523857</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C100" t="n">
+        <v>1</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1</v>
+      </c>
+      <c r="E100" t="n">
+        <v>4.453780638868921e-05</v>
+      </c>
+      <c r="F100" t="n">
+        <v>6.202274560928345</v>
+      </c>
+      <c r="G100" t="n">
+        <v>806.1558628019862</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C101" t="n">
+        <v>1</v>
+      </c>
+      <c r="D101" t="n">
+        <v>1</v>
+      </c>
+      <c r="E101" t="n">
+        <v>8.759414777159691e-05</v>
+      </c>
+      <c r="F101" t="n">
+        <v>6.233083963394165</v>
+      </c>
+      <c r="G101" t="n">
+        <v>802.1711289891399</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C102" t="n">
+        <v>1</v>
+      </c>
+      <c r="D102" t="n">
+        <v>1</v>
+      </c>
+      <c r="E102" t="n">
+        <v>1.451441949029686e-05</v>
+      </c>
+      <c r="F102" t="n">
+        <v>7.11626148223877</v>
+      </c>
+      <c r="G102" t="n">
+        <v>702.6161155656417</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C103" t="n">
+        <v>1</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1</v>
+      </c>
+      <c r="E103" t="n">
+        <v>4.367200645560843e-08</v>
+      </c>
+      <c r="F103" t="n">
+        <v>8.652847766876221</v>
+      </c>
+      <c r="G103" t="n">
+        <v>577.8444432063617</v>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C104" t="n">
+        <v>1</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1</v>
+      </c>
+      <c r="E104" t="n">
+        <v>3.709259344120142e-09</v>
+      </c>
+      <c r="F104" t="n">
+        <v>7.280958652496338</v>
+      </c>
+      <c r="G104" t="n">
+        <v>686.7227570761864</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C105" t="n">
+        <v>1</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1</v>
+      </c>
+      <c r="E105" t="n">
+        <v>2.420315922790905e-06</v>
+      </c>
+      <c r="F105" t="n">
+        <v>7.340949296951294</v>
+      </c>
+      <c r="G105" t="n">
+        <v>681.1108206504719</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1</v>
+      </c>
+      <c r="E106" t="n">
+        <v>1.360945475425979e-06</v>
+      </c>
+      <c r="F106" t="n">
+        <v>5.602527856826782</v>
+      </c>
+      <c r="G106" t="n">
+        <v>892.4542863106711</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C107" t="n">
+        <v>1</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>2.16004988960565e-14</v>
+      </c>
+      <c r="F107" t="n">
+        <v>5.390186786651611</v>
+      </c>
+      <c r="G107" t="n">
+        <v>927.6116390589879</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C108" t="n">
+        <v>1</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1</v>
+      </c>
+      <c r="E108" t="n">
+        <v>1.398498625349021e-05</v>
+      </c>
+      <c r="F108" t="n">
+        <v>5.382999181747437</v>
+      </c>
+      <c r="G108" t="n">
+        <v>928.8502247880508</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C109" t="n">
+        <v>1</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1</v>
+      </c>
+      <c r="E109" t="n">
+        <v>3.128124603790639e-07</v>
+      </c>
+      <c r="F109" t="n">
+        <v>7.285053491592407</v>
+      </c>
+      <c r="G109" t="n">
+        <v>686.3367586484354</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C110" t="n">
+        <v>1</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1</v>
+      </c>
+      <c r="E110" t="n">
+        <v>2.815966581692919e-06</v>
+      </c>
+      <c r="F110" t="n">
+        <v>7.341942548751831</v>
+      </c>
+      <c r="G110" t="n">
+        <v>681.0186768418702</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C111" t="n">
+        <v>1</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1</v>
+      </c>
+      <c r="E111" t="n">
+        <v>3.6178855111757e-07</v>
+      </c>
+      <c r="F111" t="n">
+        <v>7.254941701889038</v>
+      </c>
+      <c r="G111" t="n">
+        <v>689.185413950067</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C112" t="n">
+        <v>1</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1</v>
+      </c>
+      <c r="E112" t="n">
+        <v>4.744265424960759e-08</v>
+      </c>
+      <c r="F112" t="n">
+        <v>7.419799327850342</v>
+      </c>
+      <c r="G112" t="n">
+        <v>673.8726721668086</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C113" t="n">
+        <v>1</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1</v>
+      </c>
+      <c r="E113" t="n">
+        <v>5.806933586427476e-06</v>
+      </c>
+      <c r="F113" t="n">
+        <v>7.367447376251221</v>
+      </c>
+      <c r="G113" t="n">
+        <v>678.6611080680906</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C114" t="n">
+        <v>1</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1</v>
+      </c>
+      <c r="E114" t="n">
+        <v>4.546324635157362e-05</v>
+      </c>
+      <c r="F114" t="n">
+        <v>7.435576915740967</v>
+      </c>
+      <c r="G114" t="n">
+        <v>672.4427783693691</v>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C115" t="n">
+        <v>1</v>
+      </c>
+      <c r="D115" t="n">
+        <v>1</v>
+      </c>
+      <c r="E115" t="n">
+        <v>1.333935961156385e-05</v>
+      </c>
+      <c r="F115" t="n">
+        <v>7.344992399215698</v>
+      </c>
+      <c r="G115" t="n">
+        <v>680.735898451563</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C116" t="n">
+        <v>1</v>
+      </c>
+      <c r="D116" t="n">
+        <v>1</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.0001663380826357752</v>
+      </c>
+      <c r="F116" t="n">
+        <v>7.198201417922974</v>
+      </c>
+      <c r="G116" t="n">
+        <v>694.6179621412622</v>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C117" t="n">
+        <v>1</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1</v>
+      </c>
+      <c r="E117" t="n">
+        <v>7.050215117487824e-06</v>
+      </c>
+      <c r="F117" t="n">
+        <v>5.638320684432983</v>
+      </c>
+      <c r="G117" t="n">
+        <v>886.7888649548893</v>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C118" t="n">
+        <v>1</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1</v>
+      </c>
+      <c r="E118" t="n">
+        <v>6.970337562961504e-05</v>
+      </c>
+      <c r="F118" t="n">
+        <v>7.276855230331421</v>
+      </c>
+      <c r="G118" t="n">
+        <v>687.1100003692499</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C119" t="n">
+        <v>1</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1</v>
+      </c>
+      <c r="E119" t="n">
+        <v>2.962802318506874e-05</v>
+      </c>
+      <c r="F119" t="n">
+        <v>6.558893203735352</v>
+      </c>
+      <c r="G119" t="n">
+        <v>762.3237404067584</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C120" t="n">
+        <v>1</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1</v>
+      </c>
+      <c r="E120" t="n">
+        <v>3.85379207727965e-05</v>
+      </c>
+      <c r="F120" t="n">
+        <v>5.380234479904175</v>
+      </c>
+      <c r="G120" t="n">
+        <v>929.3275262770802</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C121" t="n">
+        <v>1</v>
+      </c>
+      <c r="D121" t="n">
+        <v>1</v>
+      </c>
+      <c r="E121" t="n">
+        <v>2.955071067844983e-05</v>
+      </c>
+      <c r="F121" t="n">
+        <v>6.049432039260864</v>
+      </c>
+      <c r="G121" t="n">
+        <v>826.5238732413156</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C122" t="n">
+        <v>1</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1</v>
+      </c>
+      <c r="E122" t="n">
+        <v>3.87423506253981e-06</v>
+      </c>
+      <c r="F122" t="n">
+        <v>7.366430521011353</v>
+      </c>
+      <c r="G122" t="n">
+        <v>678.7547898182768</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C123" t="n">
+        <v>1</v>
+      </c>
+      <c r="D123" t="n">
+        <v>1</v>
+      </c>
+      <c r="E123" t="n">
+        <v>5.02149123349227e-05</v>
+      </c>
+      <c r="F123" t="n">
+        <v>5.542580604553223</v>
+      </c>
+      <c r="G123" t="n">
+        <v>902.1068626214487</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0.0001379895402351394</v>
+      </c>
+      <c r="F124" t="n">
+        <v>5.494680166244507</v>
+      </c>
+      <c r="G124" t="n">
+        <v>909.9710717862201</v>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C125" t="n">
+        <v>1</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1</v>
+      </c>
+      <c r="E125" t="n">
+        <v>8.544651791453362e-06</v>
+      </c>
+      <c r="F125" t="n">
+        <v>7.341310501098633</v>
+      </c>
+      <c r="G125" t="n">
+        <v>681.077308915315</v>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C126" t="n">
+        <v>1</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1</v>
+      </c>
+      <c r="E126" t="n">
+        <v>1.413751760992454e-06</v>
+      </c>
+      <c r="F126" t="n">
+        <v>5.457339286804199</v>
+      </c>
+      <c r="G126" t="n">
+        <v>916.1973880000385</v>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C127" t="n">
+        <v>1</v>
+      </c>
+      <c r="D127" t="n">
+        <v>1</v>
+      </c>
+      <c r="E127" t="n">
+        <v>6.251309969229624e-05</v>
+      </c>
+      <c r="F127" t="n">
+        <v>7.343571424484253</v>
+      </c>
+      <c r="G127" t="n">
+        <v>680.8676202602817</v>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C128" t="n">
+        <v>1</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1</v>
+      </c>
+      <c r="E128" t="n">
+        <v>5.323118834610341e-09</v>
+      </c>
+      <c r="F128" t="n">
+        <v>7.236032485961914</v>
+      </c>
+      <c r="G128" t="n">
+        <v>690.9863947819646</v>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C129" t="n">
+        <v>1</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1</v>
+      </c>
+      <c r="E129" t="n">
+        <v>3.79361085833807e-06</v>
+      </c>
+      <c r="F129" t="n">
+        <v>5.460649490356445</v>
+      </c>
+      <c r="G129" t="n">
+        <v>915.6419962185897</v>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C130" t="n">
+        <v>1</v>
+      </c>
+      <c r="D130" t="n">
+        <v>1</v>
+      </c>
+      <c r="E130" t="n">
+        <v>3.932902836822905e-05</v>
+      </c>
+      <c r="F130" t="n">
+        <v>5.45056414604187</v>
+      </c>
+      <c r="G130" t="n">
+        <v>917.3362364024164</v>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C131" t="n">
+        <v>1</v>
+      </c>
+      <c r="D131" t="n">
+        <v>0</v>
+      </c>
+      <c r="E131" t="n">
+        <v>3.134779035462998e-05</v>
+      </c>
+      <c r="F131" t="n">
+        <v>4.271280765533447</v>
+      </c>
+      <c r="G131" t="n">
+        <v>1170.609068911334</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C132" t="n">
+        <v>1</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0</v>
+      </c>
+      <c r="E132" t="n">
+        <v>1.333546554432852e-12</v>
+      </c>
+      <c r="F132" t="n">
+        <v>5.113616466522217</v>
+      </c>
+      <c r="G132" t="n">
+        <v>977.7815823173208</v>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C133" t="n">
+        <v>1</v>
+      </c>
+      <c r="D133" t="n">
+        <v>1</v>
+      </c>
+      <c r="E133" t="n">
+        <v>2.690218570933212e-05</v>
+      </c>
+      <c r="F133" t="n">
+        <v>5.137114524841309</v>
+      </c>
+      <c r="G133" t="n">
+        <v>973.3090387262596</v>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 2.0</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C134" t="n">
+        <v>1</v>
+      </c>
+      <c r="D134" t="n">
+        <v>1</v>
+      </c>
+      <c r="E134" t="n">
+        <v>1.19610683668725e-06</v>
+      </c>
+      <c r="F134" t="n">
+        <v>5.913042545318604</v>
+      </c>
+      <c r="G134" t="n">
+        <v>845.5883687085144</v>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2)</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C135" t="n">
+        <v>1</v>
+      </c>
+      <c r="D135" t="n">
+        <v>1</v>
+      </c>
+      <c r="E135" t="n">
+        <v>6.999015022302046e-05</v>
+      </c>
+      <c r="F135" t="n">
+        <v>5.541564464569092</v>
+      </c>
+      <c r="G135" t="n">
+        <v>902.272279239613</v>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2)</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C136" t="n">
+        <v>1</v>
+      </c>
+      <c r="D136" t="n">
+        <v>1</v>
+      </c>
+      <c r="E136" t="n">
+        <v>7.563274721178459e-06</v>
+      </c>
+      <c r="F136" t="n">
+        <v>5.648999691009521</v>
+      </c>
+      <c r="G136" t="n">
+        <v>885.1124576900907</v>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C137" t="n">
+        <v>1</v>
+      </c>
+      <c r="D137" t="n">
+        <v>1</v>
+      </c>
+      <c r="E137" t="n">
+        <v>6.563427177752601e-06</v>
+      </c>
+      <c r="F137" t="n">
+        <v>6.243058204650879</v>
+      </c>
+      <c r="G137" t="n">
+        <v>800.8895378029889</v>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Disabled param_init for presentation.
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -5059,6 +5059,41 @@
         </is>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C138" t="n">
+        <v>1</v>
+      </c>
+      <c r="D138" t="n">
+        <v>1</v>
+      </c>
+      <c r="E138" t="n">
+        <v>1.492357114329934e-06</v>
+      </c>
+      <c r="F138" t="n">
+        <v>7.294821739196777</v>
+      </c>
+      <c r="G138" t="n">
+        <v>685.417708445682</v>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added contour plot and grid option for generators
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="experiments.csv" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="experiments.csv" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -5094,6 +5094,4066 @@
         </is>
       </c>
     </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C139" t="n">
+        <v>1</v>
+      </c>
+      <c r="D139" t="n">
+        <v>1</v>
+      </c>
+      <c r="E139" t="n">
+        <v>7.257755640921459e-08</v>
+      </c>
+      <c r="F139" t="n">
+        <v>5.636783838272095</v>
+      </c>
+      <c r="G139" t="n">
+        <v>887.0306443279728</v>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I139" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C140" t="n">
+        <v>1</v>
+      </c>
+      <c r="D140" t="n">
+        <v>1</v>
+      </c>
+      <c r="E140" t="n">
+        <v>1.929047130033723e-06</v>
+      </c>
+      <c r="F140" t="n">
+        <v>5.862632751464844</v>
+      </c>
+      <c r="G140" t="n">
+        <v>852.859152528477</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C141" t="n">
+        <v>1</v>
+      </c>
+      <c r="D141" t="n">
+        <v>1</v>
+      </c>
+      <c r="E141" t="n">
+        <v>1.579394847794902e-06</v>
+      </c>
+      <c r="F141" t="n">
+        <v>5.848613023757935</v>
+      </c>
+      <c r="G141" t="n">
+        <v>854.9035437443472</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C142" t="n">
+        <v>1</v>
+      </c>
+      <c r="D142" t="n">
+        <v>1</v>
+      </c>
+      <c r="E142" t="n">
+        <v>1.105571989512555e-08</v>
+      </c>
+      <c r="F142" t="n">
+        <v>5.33278226852417</v>
+      </c>
+      <c r="G142" t="n">
+        <v>937.5968768707547</v>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I142" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C143" t="n">
+        <v>1</v>
+      </c>
+      <c r="D143" t="n">
+        <v>1</v>
+      </c>
+      <c r="E143" t="n">
+        <v>2.967789259855635e-05</v>
+      </c>
+      <c r="F143" t="n">
+        <v>5.620429754257202</v>
+      </c>
+      <c r="G143" t="n">
+        <v>889.6116878273842</v>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C144" t="n">
+        <v>1</v>
+      </c>
+      <c r="D144" t="n">
+        <v>1</v>
+      </c>
+      <c r="E144" t="n">
+        <v>3.054315311601385e-05</v>
+      </c>
+      <c r="F144" t="n">
+        <v>5.401679515838623</v>
+      </c>
+      <c r="G144" t="n">
+        <v>925.6380326413605</v>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C145" t="n">
+        <v>1</v>
+      </c>
+      <c r="D145" t="n">
+        <v>1</v>
+      </c>
+      <c r="E145" t="n">
+        <v>5.470850510391756e-07</v>
+      </c>
+      <c r="F145" t="n">
+        <v>6.338091135025024</v>
+      </c>
+      <c r="G145" t="n">
+        <v>788.8810516417825</v>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C146" t="n">
+        <v>1</v>
+      </c>
+      <c r="D146" t="n">
+        <v>1</v>
+      </c>
+      <c r="E146" t="n">
+        <v>6.367848754962324e-07</v>
+      </c>
+      <c r="F146" t="n">
+        <v>6.005048274993896</v>
+      </c>
+      <c r="G146" t="n">
+        <v>832.6327734651029</v>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C147" t="n">
+        <v>1</v>
+      </c>
+      <c r="D147" t="n">
+        <v>1</v>
+      </c>
+      <c r="E147" t="n">
+        <v>1.437607810572672e-08</v>
+      </c>
+      <c r="F147" t="n">
+        <v>5.432624101638794</v>
+      </c>
+      <c r="G147" t="n">
+        <v>920.3655372532972</v>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C148" t="n">
+        <v>1</v>
+      </c>
+      <c r="D148" t="n">
+        <v>1</v>
+      </c>
+      <c r="E148" t="n">
+        <v>1.04908757236899e-07</v>
+      </c>
+      <c r="F148" t="n">
+        <v>5.646748065948486</v>
+      </c>
+      <c r="G148" t="n">
+        <v>885.4653938169187</v>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C149" t="n">
+        <v>1</v>
+      </c>
+      <c r="D149" t="n">
+        <v>1</v>
+      </c>
+      <c r="E149" t="n">
+        <v>8.444035159982377e-08</v>
+      </c>
+      <c r="F149" t="n">
+        <v>6.851866722106934</v>
+      </c>
+      <c r="G149" t="n">
+        <v>729.7281460347074</v>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C150" t="n">
+        <v>1</v>
+      </c>
+      <c r="D150" t="n">
+        <v>1</v>
+      </c>
+      <c r="E150" t="n">
+        <v>1.660011002968531e-05</v>
+      </c>
+      <c r="F150" t="n">
+        <v>5.278985023498535</v>
+      </c>
+      <c r="G150" t="n">
+        <v>947.1517683310941</v>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1</v>
+      </c>
+      <c r="D151" t="n">
+        <v>1</v>
+      </c>
+      <c r="E151" t="n">
+        <v>2.267540537559398e-07</v>
+      </c>
+      <c r="F151" t="n">
+        <v>5.516197919845581</v>
+      </c>
+      <c r="G151" t="n">
+        <v>906.4214287909323</v>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C152" t="n">
+        <v>1</v>
+      </c>
+      <c r="D152" t="n">
+        <v>1</v>
+      </c>
+      <c r="E152" t="n">
+        <v>2.806217935358291e-06</v>
+      </c>
+      <c r="F152" t="n">
+        <v>6.042375802993774</v>
+      </c>
+      <c r="G152" t="n">
+        <v>827.48908095433</v>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C153" t="n">
+        <v>1</v>
+      </c>
+      <c r="D153" t="n">
+        <v>1</v>
+      </c>
+      <c r="E153" t="n">
+        <v>1.723734754932593e-07</v>
+      </c>
+      <c r="F153" t="n">
+        <v>5.905207633972168</v>
+      </c>
+      <c r="G153" t="n">
+        <v>846.7102784388844</v>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>sqrt(max(abs(x) - 0.5,0)**2 + max(abs(y)- 0.5,0)**2)</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C154" t="n">
+        <v>1</v>
+      </c>
+      <c r="D154" t="n">
+        <v>1</v>
+      </c>
+      <c r="E154" t="n">
+        <v>5.601737029792275e-07</v>
+      </c>
+      <c r="F154" t="n">
+        <v>5.781871795654297</v>
+      </c>
+      <c r="G154" t="n">
+        <v>864.7718553285879</v>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C155" t="n">
+        <v>1</v>
+      </c>
+      <c r="D155" t="n">
+        <v>1</v>
+      </c>
+      <c r="E155" t="n">
+        <v>4.782774340128526e-05</v>
+      </c>
+      <c r="F155" t="n">
+        <v>7.573950052261353</v>
+      </c>
+      <c r="G155" t="n">
+        <v>660.1575090275584</v>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C156" t="n">
+        <v>16</v>
+      </c>
+      <c r="D156" t="n">
+        <v>16</v>
+      </c>
+      <c r="E156" t="n">
+        <v>0.0002763011434581131</v>
+      </c>
+      <c r="F156" t="n">
+        <v>41.63121891021729</v>
+      </c>
+      <c r="G156" t="n">
+        <v>120.1021764648088</v>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C157" t="n">
+        <v>16</v>
+      </c>
+      <c r="D157" t="n">
+        <v>16</v>
+      </c>
+      <c r="E157" t="n">
+        <v>0.0002445501449983567</v>
+      </c>
+      <c r="F157" t="n">
+        <v>41.54483675956726</v>
+      </c>
+      <c r="G157" t="n">
+        <v>120.3518990563505</v>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C158" t="n">
+        <v>1</v>
+      </c>
+      <c r="D158" t="n">
+        <v>1</v>
+      </c>
+      <c r="E158" t="n">
+        <v>1.970287712538266e-06</v>
+      </c>
+      <c r="F158" t="n">
+        <v>7.054269552230835</v>
+      </c>
+      <c r="G158" t="n">
+        <v>708.7906073023258</v>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C159" t="n">
+        <v>1</v>
+      </c>
+      <c r="D159" t="n">
+        <v>1</v>
+      </c>
+      <c r="E159" t="n">
+        <v>1.378238039251301e-06</v>
+      </c>
+      <c r="F159" t="n">
+        <v>5.270986080169678</v>
+      </c>
+      <c r="G159" t="n">
+        <v>948.589111022476</v>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C160" t="n">
+        <v>1</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1</v>
+      </c>
+      <c r="E160" t="n">
+        <v>2.176465568481945e-05</v>
+      </c>
+      <c r="F160" t="n">
+        <v>5.624000310897827</v>
+      </c>
+      <c r="G160" t="n">
+        <v>889.0468925315172</v>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C161" t="n">
+        <v>1</v>
+      </c>
+      <c r="D161" t="n">
+        <v>1</v>
+      </c>
+      <c r="E161" t="n">
+        <v>1.196512130263727e-05</v>
+      </c>
+      <c r="F161" t="n">
+        <v>5.695398569107056</v>
+      </c>
+      <c r="G161" t="n">
+        <v>877.9016849006789</v>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C162" t="n">
+        <v>1</v>
+      </c>
+      <c r="D162" t="n">
+        <v>1</v>
+      </c>
+      <c r="E162" t="n">
+        <v>2.784000798783381e-06</v>
+      </c>
+      <c r="F162" t="n">
+        <v>6.24170708656311</v>
+      </c>
+      <c r="G162" t="n">
+        <v>801.0629032502653</v>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C163" t="n">
+        <v>1</v>
+      </c>
+      <c r="D163" t="n">
+        <v>1</v>
+      </c>
+      <c r="E163" t="n">
+        <v>5.273200542887935e-08</v>
+      </c>
+      <c r="F163" t="n">
+        <v>5.746090173721313</v>
+      </c>
+      <c r="G163" t="n">
+        <v>870.1568977922728</v>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C164" t="n">
+        <v>1</v>
+      </c>
+      <c r="D164" t="n">
+        <v>1</v>
+      </c>
+      <c r="E164" t="n">
+        <v>4.310449639888247e-06</v>
+      </c>
+      <c r="F164" t="n">
+        <v>5.608452320098877</v>
+      </c>
+      <c r="G164" t="n">
+        <v>891.5115462569984</v>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C165" t="n">
+        <v>1</v>
+      </c>
+      <c r="D165" t="n">
+        <v>1</v>
+      </c>
+      <c r="E165" t="n">
+        <v>1.361301315228047e-06</v>
+      </c>
+      <c r="F165" t="n">
+        <v>5.585006237030029</v>
+      </c>
+      <c r="G165" t="n">
+        <v>895.2541479450305</v>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C166" t="n">
+        <v>1</v>
+      </c>
+      <c r="D166" t="n">
+        <v>1</v>
+      </c>
+      <c r="E166" t="n">
+        <v>1.951627887075702e-10</v>
+      </c>
+      <c r="F166" t="n">
+        <v>5.644744873046875</v>
+      </c>
+      <c r="G166" t="n">
+        <v>885.7796255548287</v>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C167" t="n">
+        <v>1</v>
+      </c>
+      <c r="D167" t="n">
+        <v>1</v>
+      </c>
+      <c r="E167" t="n">
+        <v>1.151450823577704e-09</v>
+      </c>
+      <c r="F167" t="n">
+        <v>7.655393362045288</v>
+      </c>
+      <c r="G167" t="n">
+        <v>653.1343019928308</v>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C168" t="n">
+        <v>1</v>
+      </c>
+      <c r="D168" t="n">
+        <v>1</v>
+      </c>
+      <c r="E168" t="n">
+        <v>1.174385133410893e-12</v>
+      </c>
+      <c r="F168" t="n">
+        <v>7.124485731124878</v>
+      </c>
+      <c r="G168" t="n">
+        <v>701.805040910729</v>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C169" t="n">
+        <v>1</v>
+      </c>
+      <c r="D169" t="n">
+        <v>1</v>
+      </c>
+      <c r="E169" t="n">
+        <v>2.942125547633623e-06</v>
+      </c>
+      <c r="F169" t="n">
+        <v>5.452187299728394</v>
+      </c>
+      <c r="G169" t="n">
+        <v>917.063139090816</v>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C170" t="n">
+        <v>1</v>
+      </c>
+      <c r="D170" t="n">
+        <v>1</v>
+      </c>
+      <c r="E170" t="n">
+        <v>8.959887519421894e-12</v>
+      </c>
+      <c r="F170" t="n">
+        <v>6.957131147384644</v>
+      </c>
+      <c r="G170" t="n">
+        <v>718.6870412640737</v>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C171" t="n">
+        <v>1</v>
+      </c>
+      <c r="D171" t="n">
+        <v>1</v>
+      </c>
+      <c r="E171" t="n">
+        <v>6.217915142769925e-06</v>
+      </c>
+      <c r="F171" t="n">
+        <v>5.362480878829956</v>
+      </c>
+      <c r="G171" t="n">
+        <v>932.4042570928391</v>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C172" t="n">
+        <v>1</v>
+      </c>
+      <c r="D172" t="n">
+        <v>1</v>
+      </c>
+      <c r="E172" t="n">
+        <v>1.707576408830486e-13</v>
+      </c>
+      <c r="F172" t="n">
+        <v>4.963119268417358</v>
+      </c>
+      <c r="G172" t="n">
+        <v>1007.430958151123</v>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C173" t="n">
+        <v>1</v>
+      </c>
+      <c r="D173" t="n">
+        <v>1</v>
+      </c>
+      <c r="E173" t="n">
+        <v>2.777491317829117e-06</v>
+      </c>
+      <c r="F173" t="n">
+        <v>5.734473705291748</v>
+      </c>
+      <c r="G173" t="n">
+        <v>871.9195966294207</v>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I173" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C174" t="n">
+        <v>1</v>
+      </c>
+      <c r="D174" t="n">
+        <v>1</v>
+      </c>
+      <c r="E174" t="n">
+        <v>1.630268542385238e-08</v>
+      </c>
+      <c r="F174" t="n">
+        <v>5.984594583511353</v>
+      </c>
+      <c r="G174" t="n">
+        <v>835.4784823312693</v>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I174" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C175" t="n">
+        <v>1</v>
+      </c>
+      <c r="D175" t="n">
+        <v>1</v>
+      </c>
+      <c r="E175" t="n">
+        <v>2.251372421824271e-10</v>
+      </c>
+      <c r="F175" t="n">
+        <v>4.916674375534058</v>
+      </c>
+      <c r="G175" t="n">
+        <v>1016.947558064976</v>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I175" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C176" t="n">
+        <v>1</v>
+      </c>
+      <c r="D176" t="n">
+        <v>1</v>
+      </c>
+      <c r="E176" t="n">
+        <v>6.15848136931163e-08</v>
+      </c>
+      <c r="F176" t="n">
+        <v>5.085296392440796</v>
+      </c>
+      <c r="G176" t="n">
+        <v>983.2268591920055</v>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I176" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C177" t="n">
+        <v>1</v>
+      </c>
+      <c r="D177" t="n">
+        <v>1</v>
+      </c>
+      <c r="E177" t="n">
+        <v>1.991829590153316e-09</v>
+      </c>
+      <c r="F177" t="n">
+        <v>5.19362998008728</v>
+      </c>
+      <c r="G177" t="n">
+        <v>962.7177945233545</v>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1</v>
+      </c>
+      <c r="D178" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" t="n">
+        <v>1.935632210070537e-12</v>
+      </c>
+      <c r="F178" t="n">
+        <v>5.091040372848511</v>
+      </c>
+      <c r="G178" t="n">
+        <v>982.1175307636438</v>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C179" t="n">
+        <v>1</v>
+      </c>
+      <c r="D179" t="n">
+        <v>1</v>
+      </c>
+      <c r="E179" t="n">
+        <v>3.178158976879786e-06</v>
+      </c>
+      <c r="F179" t="n">
+        <v>5.46095085144043</v>
+      </c>
+      <c r="G179" t="n">
+        <v>915.5914667646487</v>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C180" t="n">
+        <v>1</v>
+      </c>
+      <c r="D180" t="n">
+        <v>1</v>
+      </c>
+      <c r="E180" t="n">
+        <v>8.201575529831473e-10</v>
+      </c>
+      <c r="F180" t="n">
+        <v>5.320547103881836</v>
+      </c>
+      <c r="G180" t="n">
+        <v>939.7529807323824</v>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1</v>
+      </c>
+      <c r="D181" t="n">
+        <v>1</v>
+      </c>
+      <c r="E181" t="n">
+        <v>5.465927016556904e-11</v>
+      </c>
+      <c r="F181" t="n">
+        <v>5.483335018157959</v>
+      </c>
+      <c r="G181" t="n">
+        <v>911.8538231646609</v>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C182" t="n">
+        <v>1</v>
+      </c>
+      <c r="D182" t="n">
+        <v>1</v>
+      </c>
+      <c r="E182" t="n">
+        <v>8.850436827856356e-09</v>
+      </c>
+      <c r="F182" t="n">
+        <v>6.06887412071228</v>
+      </c>
+      <c r="G182" t="n">
+        <v>823.8760436529155</v>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C183" t="n">
+        <v>1</v>
+      </c>
+      <c r="D183" t="n">
+        <v>1</v>
+      </c>
+      <c r="E183" t="n">
+        <v>3.351488195042079e-13</v>
+      </c>
+      <c r="F183" t="n">
+        <v>5.181371212005615</v>
+      </c>
+      <c r="G183" t="n">
+        <v>964.9955186408253</v>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C184" t="n">
+        <v>1</v>
+      </c>
+      <c r="D184" t="n">
+        <v>1</v>
+      </c>
+      <c r="E184" t="n">
+        <v>6.330856672231988e-11</v>
+      </c>
+      <c r="F184" t="n">
+        <v>5.494903802871704</v>
+      </c>
+      <c r="G184" t="n">
+        <v>909.9340369501899</v>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C185" t="n">
+        <v>1</v>
+      </c>
+      <c r="D185" t="n">
+        <v>1</v>
+      </c>
+      <c r="E185" t="n">
+        <v>3.006735527222304e-09</v>
+      </c>
+      <c r="F185" t="n">
+        <v>5.538063526153564</v>
+      </c>
+      <c r="G185" t="n">
+        <v>902.8426590607793</v>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C186" t="n">
+        <v>1</v>
+      </c>
+      <c r="D186" t="n">
+        <v>1</v>
+      </c>
+      <c r="E186" t="n">
+        <v>4.766475467476994e-05</v>
+      </c>
+      <c r="F186" t="n">
+        <v>5.544052362442017</v>
+      </c>
+      <c r="G186" t="n">
+        <v>901.8673838422451</v>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C187" t="n">
+        <v>1</v>
+      </c>
+      <c r="D187" t="n">
+        <v>1</v>
+      </c>
+      <c r="E187" t="n">
+        <v>4.812818980154399e-12</v>
+      </c>
+      <c r="F187" t="n">
+        <v>6.002375841140747</v>
+      </c>
+      <c r="G187" t="n">
+        <v>833.0034860079261</v>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C188" t="n">
+        <v>1</v>
+      </c>
+      <c r="D188" t="n">
+        <v>1</v>
+      </c>
+      <c r="E188" t="n">
+        <v>2.013808625633828e-05</v>
+      </c>
+      <c r="F188" t="n">
+        <v>5.530017375946045</v>
+      </c>
+      <c r="G188" t="n">
+        <v>904.1562910359984</v>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C189" t="n">
+        <v>1</v>
+      </c>
+      <c r="D189" t="n">
+        <v>1</v>
+      </c>
+      <c r="E189" t="n">
+        <v>4.050889398227175e-12</v>
+      </c>
+      <c r="F189" t="n">
+        <v>6.540792465209961</v>
+      </c>
+      <c r="G189" t="n">
+        <v>764.4333659254083</v>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C190" t="n">
+        <v>1</v>
+      </c>
+      <c r="D190" t="n">
+        <v>1</v>
+      </c>
+      <c r="E190" t="n">
+        <v>8.27976577966183e-07</v>
+      </c>
+      <c r="F190" t="n">
+        <v>6.626197814941406</v>
+      </c>
+      <c r="G190" t="n">
+        <v>754.580551266596</v>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C191" t="n">
+        <v>1</v>
+      </c>
+      <c r="D191" t="n">
+        <v>1</v>
+      </c>
+      <c r="E191" t="n">
+        <v>1.589310727467819e-08</v>
+      </c>
+      <c r="F191" t="n">
+        <v>6.305509805679321</v>
+      </c>
+      <c r="G191" t="n">
+        <v>792.9572951415507</v>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C192" t="n">
+        <v>1</v>
+      </c>
+      <c r="D192" t="n">
+        <v>1</v>
+      </c>
+      <c r="E192" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F192" t="n">
+        <v>5.37976336479187</v>
+      </c>
+      <c r="G192" t="n">
+        <v>929.4089090837618</v>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I192" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C193" t="n">
+        <v>1</v>
+      </c>
+      <c r="D193" t="n">
+        <v>1</v>
+      </c>
+      <c r="E193" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F193" t="n">
+        <v>5.315362691879272</v>
+      </c>
+      <c r="G193" t="n">
+        <v>940.6695817086803</v>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C194" t="n">
+        <v>1</v>
+      </c>
+      <c r="D194" t="n">
+        <v>1</v>
+      </c>
+      <c r="E194" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F194" t="n">
+        <v>5.281413555145264</v>
+      </c>
+      <c r="G194" t="n">
+        <v>946.7162432544021</v>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C195" t="n">
+        <v>1</v>
+      </c>
+      <c r="D195" t="n">
+        <v>1</v>
+      </c>
+      <c r="E195" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F195" t="n">
+        <v>6.538342475891113</v>
+      </c>
+      <c r="G195" t="n">
+        <v>764.7198075714974</v>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C196" t="n">
+        <v>1</v>
+      </c>
+      <c r="D196" t="n">
+        <v>1</v>
+      </c>
+      <c r="E196" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F196" t="n">
+        <v>6.969060182571411</v>
+      </c>
+      <c r="G196" t="n">
+        <v>717.4568548718033</v>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C197" t="n">
+        <v>1</v>
+      </c>
+      <c r="D197" t="n">
+        <v>1</v>
+      </c>
+      <c r="E197" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F197" t="n">
+        <v>5.130970239639282</v>
+      </c>
+      <c r="G197" t="n">
+        <v>974.474566500606</v>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I197" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C198" t="n">
+        <v>1</v>
+      </c>
+      <c r="D198" t="n">
+        <v>1</v>
+      </c>
+      <c r="E198" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F198" t="n">
+        <v>7.032819986343384</v>
+      </c>
+      <c r="G198" t="n">
+        <v>710.9523647284025</v>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C199" t="n">
+        <v>1</v>
+      </c>
+      <c r="D199" t="n">
+        <v>1</v>
+      </c>
+      <c r="E199" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F199" t="n">
+        <v>5.986383676528931</v>
+      </c>
+      <c r="G199" t="n">
+        <v>835.2287908982033</v>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C200" t="n">
+        <v>1</v>
+      </c>
+      <c r="D200" t="n">
+        <v>1</v>
+      </c>
+      <c r="E200" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F200" t="n">
+        <v>6.087401151657104</v>
+      </c>
+      <c r="G200" t="n">
+        <v>821.3685734574773</v>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C201" t="n">
+        <v>1</v>
+      </c>
+      <c r="D201" t="n">
+        <v>1</v>
+      </c>
+      <c r="E201" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F201" t="n">
+        <v>5.049807786941528</v>
+      </c>
+      <c r="G201" t="n">
+        <v>990.136696475789</v>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C202" t="n">
+        <v>1</v>
+      </c>
+      <c r="D202" t="n">
+        <v>1</v>
+      </c>
+      <c r="E202" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F202" t="n">
+        <v>5.049566030502319</v>
+      </c>
+      <c r="G202" t="n">
+        <v>990.1841009300776</v>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C203" t="n">
+        <v>1</v>
+      </c>
+      <c r="D203" t="n">
+        <v>1</v>
+      </c>
+      <c r="E203" t="n">
+        <v>9.30413125016516e-12</v>
+      </c>
+      <c r="F203" t="n">
+        <v>5.320998668670654</v>
+      </c>
+      <c r="G203" t="n">
+        <v>939.6732289070748</v>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C204" t="n">
+        <v>1</v>
+      </c>
+      <c r="D204" t="n">
+        <v>0</v>
+      </c>
+      <c r="E204" t="n">
+        <v>0</v>
+      </c>
+      <c r="F204" t="n">
+        <v>3.981000185012817</v>
+      </c>
+      <c r="G204" t="n">
+        <v>1255.965779359516</v>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C205" t="n">
+        <v>1</v>
+      </c>
+      <c r="D205" t="n">
+        <v>0</v>
+      </c>
+      <c r="E205" t="n">
+        <v>0</v>
+      </c>
+      <c r="F205" t="n">
+        <v>4.004102230072021</v>
+      </c>
+      <c r="G205" t="n">
+        <v>1248.719366465842</v>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C206" t="n">
+        <v>16</v>
+      </c>
+      <c r="D206" t="n">
+        <v>16</v>
+      </c>
+      <c r="E206" t="n">
+        <v>2.79639529310316e-08</v>
+      </c>
+      <c r="F206" t="n">
+        <v>214.0385761260986</v>
+      </c>
+      <c r="G206" t="n">
+        <v>93.44110002029356</v>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C207" t="n">
+        <v>1</v>
+      </c>
+      <c r="D207" t="n">
+        <v>0</v>
+      </c>
+      <c r="E207" t="n">
+        <v>0</v>
+      </c>
+      <c r="F207" t="n">
+        <v>19.25755190849304</v>
+      </c>
+      <c r="G207" t="n">
+        <v>1038.553607178881</v>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C208" t="n">
+        <v>2</v>
+      </c>
+      <c r="D208" t="n">
+        <v>2</v>
+      </c>
+      <c r="E208" t="n">
+        <v>5.674564984570196e-12</v>
+      </c>
+      <c r="F208" t="n">
+        <v>42.51690006256104</v>
+      </c>
+      <c r="G208" t="n">
+        <v>470.4011809556015</v>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I208" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C209" t="n">
+        <v>2</v>
+      </c>
+      <c r="D209" t="n">
+        <v>2</v>
+      </c>
+      <c r="E209" t="n">
+        <v>5.674564984570196e-12</v>
+      </c>
+      <c r="F209" t="n">
+        <v>43.11398983001709</v>
+      </c>
+      <c r="G209" t="n">
+        <v>463.8865500236184</v>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C210" t="n">
+        <v>1</v>
+      </c>
+      <c r="D210" t="n">
+        <v>1</v>
+      </c>
+      <c r="E210" t="n">
+        <v>2.162182793918888e-10</v>
+      </c>
+      <c r="F210" t="n">
+        <v>4.948001623153687</v>
+      </c>
+      <c r="G210" t="n">
+        <v>1010.508965195766</v>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C211" t="n">
+        <v>2</v>
+      </c>
+      <c r="D211" t="n">
+        <v>2</v>
+      </c>
+      <c r="E211" t="n">
+        <v>0.0001427740207873285</v>
+      </c>
+      <c r="F211" t="n">
+        <v>30.28485465049744</v>
+      </c>
+      <c r="G211" t="n">
+        <v>660.3961032935482</v>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C212" t="n">
+        <v>2</v>
+      </c>
+      <c r="D212" t="n">
+        <v>2</v>
+      </c>
+      <c r="E212" t="n">
+        <v>1.295797301281709e-05</v>
+      </c>
+      <c r="F212" t="n">
+        <v>34.2751452922821</v>
+      </c>
+      <c r="G212" t="n">
+        <v>583.5132084619783</v>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C213" t="n">
+        <v>2</v>
+      </c>
+      <c r="D213" t="n">
+        <v>2</v>
+      </c>
+      <c r="E213" t="n">
+        <v>1.295797301281709e-05</v>
+      </c>
+      <c r="F213" t="n">
+        <v>29.36824917793274</v>
+      </c>
+      <c r="G213" t="n">
+        <v>681.007569733778</v>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C214" t="n">
+        <v>1</v>
+      </c>
+      <c r="D214" t="n">
+        <v>1</v>
+      </c>
+      <c r="E214" t="n">
+        <v>5.795648405637621e-09</v>
+      </c>
+      <c r="F214" t="n">
+        <v>6.774195909500122</v>
+      </c>
+      <c r="G214" t="n">
+        <v>738.094980835734</v>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B215" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C215" t="n">
+        <v>1</v>
+      </c>
+      <c r="D215" t="n">
+        <v>1</v>
+      </c>
+      <c r="E215" t="n">
+        <v>5.795648405637621e-09</v>
+      </c>
+      <c r="F215" t="n">
+        <v>5.154603481292725</v>
+      </c>
+      <c r="G215" t="n">
+        <v>970.0067169368474</v>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C216" t="n">
+        <v>1</v>
+      </c>
+      <c r="D216" t="n">
+        <v>1</v>
+      </c>
+      <c r="E216" t="n">
+        <v>5.795648405637621e-09</v>
+      </c>
+      <c r="F216" t="n">
+        <v>5.250000476837158</v>
+      </c>
+      <c r="G216" t="n">
+        <v>952.3808658798885</v>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C217" t="n">
+        <v>1</v>
+      </c>
+      <c r="D217" t="n">
+        <v>1</v>
+      </c>
+      <c r="E217" t="n">
+        <v>5.795648405637621e-09</v>
+      </c>
+      <c r="F217" t="n">
+        <v>5.360483646392822</v>
+      </c>
+      <c r="G217" t="n">
+        <v>932.7516563481358</v>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C218" t="n">
+        <v>1</v>
+      </c>
+      <c r="D218" t="n">
+        <v>0</v>
+      </c>
+      <c r="E218" t="n">
+        <v>0</v>
+      </c>
+      <c r="F218" t="n">
+        <v>5.200076818466187</v>
+      </c>
+      <c r="G218" t="n">
+        <v>961.5242571502624</v>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C219" t="n">
+        <v>1</v>
+      </c>
+      <c r="D219" t="n">
+        <v>0</v>
+      </c>
+      <c r="E219" t="n">
+        <v>0</v>
+      </c>
+      <c r="F219" t="n">
+        <v>4.055082559585571</v>
+      </c>
+      <c r="G219" t="n">
+        <v>1233.020518455486</v>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C220" t="n">
+        <v>1</v>
+      </c>
+      <c r="D220" t="n">
+        <v>0</v>
+      </c>
+      <c r="E220" t="n">
+        <v>0</v>
+      </c>
+      <c r="F220" t="n">
+        <v>4.49811577796936</v>
+      </c>
+      <c r="G220" t="n">
+        <v>1111.576546003716</v>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C221" t="n">
+        <v>1</v>
+      </c>
+      <c r="D221" t="n">
+        <v>0</v>
+      </c>
+      <c r="E221" t="n">
+        <v>0</v>
+      </c>
+      <c r="F221" t="n">
+        <v>3.875794410705566</v>
+      </c>
+      <c r="G221" t="n">
+        <v>1290.058106846224</v>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C222" t="n">
+        <v>1</v>
+      </c>
+      <c r="D222" t="n">
+        <v>0</v>
+      </c>
+      <c r="E222" t="n">
+        <v>0</v>
+      </c>
+      <c r="F222" t="n">
+        <v>3.827111959457397</v>
+      </c>
+      <c r="G222" t="n">
+        <v>1306.468180959329</v>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C223" t="n">
+        <v>1</v>
+      </c>
+      <c r="D223" t="n">
+        <v>1</v>
+      </c>
+      <c r="E223" t="n">
+        <v>0</v>
+      </c>
+      <c r="F223" t="n">
+        <v>4.501964330673218</v>
+      </c>
+      <c r="G223" t="n">
+        <v>1110.626302819309</v>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C224" t="n">
+        <v>16</v>
+      </c>
+      <c r="D224" t="n">
+        <v>16</v>
+      </c>
+      <c r="E224" t="n">
+        <v>2.190240138588706e-06</v>
+      </c>
+      <c r="F224" t="n">
+        <v>34.08241629600525</v>
+      </c>
+      <c r="G224" t="n">
+        <v>146.7032136622908</v>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I224" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C225" t="n">
+        <v>16</v>
+      </c>
+      <c r="D225" t="n">
+        <v>16</v>
+      </c>
+      <c r="E225" t="n">
+        <v>0.0003812232753261924</v>
+      </c>
+      <c r="F225" t="n">
+        <v>131.7473182678223</v>
+      </c>
+      <c r="G225" t="n">
+        <v>151.8057465074397</v>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>50000</v>
+      </c>
+      <c r="C226" t="n">
+        <v>8</v>
+      </c>
+      <c r="D226" t="n">
+        <v>8</v>
+      </c>
+      <c r="E226" t="n">
+        <v>8.924961730372161e-05</v>
+      </c>
+      <c r="F226" t="n">
+        <v>173.6839334964752</v>
+      </c>
+      <c r="G226" t="n">
+        <v>287.8792470520292</v>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>50000</v>
+      </c>
+      <c r="C227" t="n">
+        <v>8</v>
+      </c>
+      <c r="D227" t="n">
+        <v>8</v>
+      </c>
+      <c r="E227" t="n">
+        <v>6.501793541247025e-05</v>
+      </c>
+      <c r="F227" t="n">
+        <v>181.0770690441132</v>
+      </c>
+      <c r="G227" t="n">
+        <v>276.1255208290302</v>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C228" t="n">
+        <v>1</v>
+      </c>
+      <c r="D228" t="n">
+        <v>1</v>
+      </c>
+      <c r="E228" t="n">
+        <v>3.659739455930122e-10</v>
+      </c>
+      <c r="F228" t="n">
+        <v>4.686026096343994</v>
+      </c>
+      <c r="G228" t="n">
+        <v>1067.002167124286</v>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B229" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C229" t="n">
+        <v>1</v>
+      </c>
+      <c r="D229" t="n">
+        <v>1</v>
+      </c>
+      <c r="E229" t="n">
+        <v>3.659739455930122e-10</v>
+      </c>
+      <c r="F229" t="n">
+        <v>6.5269775390625</v>
+      </c>
+      <c r="G229" t="n">
+        <v>766.0513568609849</v>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B230" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C230" t="n">
+        <v>8</v>
+      </c>
+      <c r="D230" t="n">
+        <v>8</v>
+      </c>
+      <c r="E230" t="n">
+        <v>3.133235168206738e-06</v>
+      </c>
+      <c r="F230" t="n">
+        <v>70.44143176078796</v>
+      </c>
+      <c r="G230" t="n">
+        <v>283.9238144380425</v>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B231" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C231" t="n">
+        <v>8</v>
+      </c>
+      <c r="D231" t="n">
+        <v>8</v>
+      </c>
+      <c r="E231" t="n">
+        <v>3.133235168206738e-06</v>
+      </c>
+      <c r="F231" t="n">
+        <v>70.2745475769043</v>
+      </c>
+      <c r="G231" t="n">
+        <v>284.5980613124999</v>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B232" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C232" t="n">
+        <v>8</v>
+      </c>
+      <c r="D232" t="n">
+        <v>8</v>
+      </c>
+      <c r="E232" t="n">
+        <v>3.133235168206738e-06</v>
+      </c>
+      <c r="F232" t="n">
+        <v>71.29628920555115</v>
+      </c>
+      <c r="G232" t="n">
+        <v>280.5195084184381</v>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B233" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C233" t="n">
+        <v>8</v>
+      </c>
+      <c r="D233" t="n">
+        <v>8</v>
+      </c>
+      <c r="E233" t="n">
+        <v>3.133235168206738e-06</v>
+      </c>
+      <c r="F233" t="n">
+        <v>71.99184322357178</v>
+      </c>
+      <c r="G233" t="n">
+        <v>277.8092503881265</v>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B234" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C234" t="n">
+        <v>8</v>
+      </c>
+      <c r="D234" t="n">
+        <v>8</v>
+      </c>
+      <c r="E234" t="n">
+        <v>3.133235168206738e-06</v>
+      </c>
+      <c r="F234" t="n">
+        <v>72.27164554595947</v>
+      </c>
+      <c r="G234" t="n">
+        <v>276.7337017016094</v>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B235" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C235" t="n">
+        <v>8</v>
+      </c>
+      <c r="D235" t="n">
+        <v>8</v>
+      </c>
+      <c r="E235" t="n">
+        <v>3.133235168206738e-06</v>
+      </c>
+      <c r="F235" t="n">
+        <v>69.8344407081604</v>
+      </c>
+      <c r="G235" t="n">
+        <v>286.391639958576</v>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B236" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C236" t="n">
+        <v>1</v>
+      </c>
+      <c r="D236" t="n">
+        <v>1</v>
+      </c>
+      <c r="E236" t="n">
+        <v>1.239531410845984e-08</v>
+      </c>
+      <c r="F236" t="n">
+        <v>19.86653709411621</v>
+      </c>
+      <c r="G236" t="n">
+        <v>1006.71797531958</v>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B237" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C237" t="n">
+        <v>1</v>
+      </c>
+      <c r="D237" t="n">
+        <v>1</v>
+      </c>
+      <c r="E237" t="n">
+        <v>1.239531410845984e-08</v>
+      </c>
+      <c r="F237" t="n">
+        <v>23.30841422080994</v>
+      </c>
+      <c r="G237" t="n">
+        <v>858.0592317663483</v>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B238" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C238" t="n">
+        <v>1</v>
+      </c>
+      <c r="D238" t="n">
+        <v>1</v>
+      </c>
+      <c r="E238" t="n">
+        <v>1.239531410845984e-08</v>
+      </c>
+      <c r="F238" t="n">
+        <v>18.31232166290283</v>
+      </c>
+      <c r="G238" t="n">
+        <v>1092.160806705142</v>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B239" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C239" t="n">
+        <v>1</v>
+      </c>
+      <c r="D239" t="n">
+        <v>1</v>
+      </c>
+      <c r="E239" t="n">
+        <v>1.239531410845984e-08</v>
+      </c>
+      <c r="F239" t="n">
+        <v>20.31764626502991</v>
+      </c>
+      <c r="G239" t="n">
+        <v>984.3659909771817</v>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B240" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C240" t="n">
+        <v>1</v>
+      </c>
+      <c r="D240" t="n">
+        <v>1</v>
+      </c>
+      <c r="E240" t="n">
+        <v>1.239531410845984e-08</v>
+      </c>
+      <c r="F240" t="n">
+        <v>19.52239656448364</v>
+      </c>
+      <c r="G240" t="n">
+        <v>1024.464385504044</v>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B241" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C241" t="n">
+        <v>1</v>
+      </c>
+      <c r="D241" t="n">
+        <v>1</v>
+      </c>
+      <c r="E241" t="n">
+        <v>0.0534057505428791</v>
+      </c>
+      <c r="F241" t="n">
+        <v>19.75332832336426</v>
+      </c>
+      <c r="G241" t="n">
+        <v>1012.487600701902</v>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B242" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C242" t="n">
+        <v>1</v>
+      </c>
+      <c r="D242" t="n">
+        <v>1</v>
+      </c>
+      <c r="E242" t="n">
+        <v>1.596850052010268e-05</v>
+      </c>
+      <c r="F242" t="n">
+        <v>22.34767508506775</v>
+      </c>
+      <c r="G242" t="n">
+        <v>894.947681307734</v>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B243" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C243" t="n">
+        <v>1</v>
+      </c>
+      <c r="D243" t="n">
+        <v>1</v>
+      </c>
+      <c r="E243" t="n">
+        <v>1.596850052010268e-05</v>
+      </c>
+      <c r="F243" t="n">
+        <v>24.69485569000244</v>
+      </c>
+      <c r="G243" t="n">
+        <v>809.8852753408426</v>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I243" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B244" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C244" t="n">
+        <v>1</v>
+      </c>
+      <c r="D244" t="n">
+        <v>1</v>
+      </c>
+      <c r="E244" t="n">
+        <v>1.596850052010268e-05</v>
+      </c>
+      <c r="F244" t="n">
+        <v>23.00197601318359</v>
+      </c>
+      <c r="G244" t="n">
+        <v>869.4905163163804</v>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B245" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C245" t="n">
+        <v>1</v>
+      </c>
+      <c r="D245" t="n">
+        <v>1</v>
+      </c>
+      <c r="E245" t="n">
+        <v>1.596850052010268e-05</v>
+      </c>
+      <c r="F245" t="n">
+        <v>22.40120530128479</v>
+      </c>
+      <c r="G245" t="n">
+        <v>892.8091025018608</v>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B246" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C246" t="n">
+        <v>1</v>
+      </c>
+      <c r="D246" t="n">
+        <v>1</v>
+      </c>
+      <c r="E246" t="n">
+        <v>1.596850052010268e-05</v>
+      </c>
+      <c r="F246" t="n">
+        <v>22.23286366462708</v>
+      </c>
+      <c r="G246" t="n">
+        <v>899.5692278642626</v>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B247" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C247" t="n">
+        <v>1</v>
+      </c>
+      <c r="D247" t="n">
+        <v>1</v>
+      </c>
+      <c r="E247" t="n">
+        <v>1.596850052010268e-05</v>
+      </c>
+      <c r="F247" t="n">
+        <v>22.68486666679382</v>
+      </c>
+      <c r="G247" t="n">
+        <v>881.6450320722431</v>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B248" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C248" t="n">
+        <v>1</v>
+      </c>
+      <c r="D248" t="n">
+        <v>1</v>
+      </c>
+      <c r="E248" t="n">
+        <v>1.596850052010268e-05</v>
+      </c>
+      <c r="F248" t="n">
+        <v>22.1418571472168</v>
+      </c>
+      <c r="G248" t="n">
+        <v>903.2665989588852</v>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B249" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C249" t="n">
+        <v>1</v>
+      </c>
+      <c r="D249" t="n">
+        <v>1</v>
+      </c>
+      <c r="E249" t="n">
+        <v>0.0002488105383235961</v>
+      </c>
+      <c r="F249" t="n">
+        <v>5.906536817550659</v>
+      </c>
+      <c r="G249" t="n">
+        <v>846.5197381218417</v>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B250" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C250" t="n">
+        <v>1</v>
+      </c>
+      <c r="D250" t="n">
+        <v>1</v>
+      </c>
+      <c r="E250" t="n">
+        <v>0.0002488105383235961</v>
+      </c>
+      <c r="F250" t="n">
+        <v>6.040567874908447</v>
+      </c>
+      <c r="G250" t="n">
+        <v>827.7367465349078</v>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B251" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C251" t="n">
+        <v>1</v>
+      </c>
+      <c r="D251" t="n">
+        <v>1</v>
+      </c>
+      <c r="E251" t="n">
+        <v>1.317470292860889e-07</v>
+      </c>
+      <c r="F251" t="n">
+        <v>7.209877967834473</v>
+      </c>
+      <c r="G251" t="n">
+        <v>693.4930136552337</v>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B252" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C252" t="n">
+        <v>1</v>
+      </c>
+      <c r="D252" t="n">
+        <v>1</v>
+      </c>
+      <c r="E252" t="n">
+        <v>0.0002488105383235961</v>
+      </c>
+      <c r="F252" t="n">
+        <v>5.441074132919312</v>
+      </c>
+      <c r="G252" t="n">
+        <v>918.936202274704</v>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B253" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C253" t="n">
+        <v>1</v>
+      </c>
+      <c r="D253" t="n">
+        <v>1</v>
+      </c>
+      <c r="E253" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F253" t="n">
+        <v>7.308667659759521</v>
+      </c>
+      <c r="G253" t="n">
+        <v>684.119217450437</v>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B254" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C254" t="n">
+        <v>1</v>
+      </c>
+      <c r="D254" t="n">
+        <v>1</v>
+      </c>
+      <c r="E254" t="n">
+        <v>1.317470292860889e-07</v>
+      </c>
+      <c r="F254" t="n">
+        <v>7.110841035842896</v>
+      </c>
+      <c r="G254" t="n">
+        <v>703.1517052338826</v>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Initialization replacement, shm and other optimizations.
</commit_message>
<xml_diff>
--- a/data/experiments.xlsx
+++ b/data/experiments.xlsx
@@ -9154,6 +9154,4498 @@
         </is>
       </c>
     </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0])*np.sqrt(np.max(np.abs(x) - 0.5,0)[0]) + np.max(np.abs(y)- 0.5,0)[0] * np.max(np.abs(y)- 0.5,0)[0]</t>
+        </is>
+      </c>
+      <c r="B255" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C255" t="n">
+        <v>1</v>
+      </c>
+      <c r="D255" t="n">
+        <v>1</v>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F255" t="n">
+        <v>6.610589981079102</v>
+      </c>
+      <c r="G255" t="n">
+        <v>756.3621423066702</v>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[0]) + np.max(np.abs(y)- 0.5,0)[0]*np.max(np.abs(y)- 0.5,0)[0]</t>
+        </is>
+      </c>
+      <c r="B256" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C256" t="n">
+        <v>1</v>
+      </c>
+      <c r="D256" t="n">
+        <v>1</v>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F256" t="n">
+        <v>7.387731313705444</v>
+      </c>
+      <c r="G256" t="n">
+        <v>676.7977593776571</v>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[0]) + np.max(np.abs(y)- 0.5,0)[0]*np.max(np.abs(y)- 0.5,0)[0]</t>
+        </is>
+      </c>
+      <c r="B257" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C257" t="n">
+        <v>1</v>
+      </c>
+      <c r="D257" t="n">
+        <v>1</v>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F257" t="n">
+        <v>6.02351975440979</v>
+      </c>
+      <c r="G257" t="n">
+        <v>830.0794558429934</v>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[0]) + np.max(np.abs(y)- 0.5,0)[0]*np.max(np.abs(y)- 0.5,0)[0]</t>
+        </is>
+      </c>
+      <c r="B258" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C258" t="n">
+        <v>1</v>
+      </c>
+      <c r="D258" t="n">
+        <v>1</v>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F258" t="n">
+        <v>5.896962404251099</v>
+      </c>
+      <c r="G258" t="n">
+        <v>847.8941626616983</v>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[0]) + np.max(np.abs(y)- 0.5,0)[0]*np.max(np.abs(y)- 0.5,0)[0]</t>
+        </is>
+      </c>
+      <c r="B259" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C259" t="n">
+        <v>2</v>
+      </c>
+      <c r="D259" t="n">
+        <v>2</v>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F259" t="n">
+        <v>8.528831958770752</v>
+      </c>
+      <c r="G259" t="n">
+        <v>586.2467479920477</v>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[0]) + np.max(np.abs(y)- 0.5,0)[0]*np.max(np.abs(y)- 0.5,0)[0]</t>
+        </is>
+      </c>
+      <c r="B260" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C260" t="n">
+        <v>2</v>
+      </c>
+      <c r="D260" t="n">
+        <v>2</v>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F260" t="n">
+        <v>10.87864327430725</v>
+      </c>
+      <c r="G260" t="n">
+        <v>459.616137226303</v>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[1]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[1]) + np.max(np.abs(y)- 0.5,0)[1]*np.max(np.abs(y)- 0.5,0)[1]</t>
+        </is>
+      </c>
+      <c r="B261" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C261" t="n">
+        <v>2</v>
+      </c>
+      <c r="D261" t="n">
+        <v>2</v>
+      </c>
+      <c r="E261" t="n">
+        <v>0.0002519141708035022</v>
+      </c>
+      <c r="F261" t="n">
+        <v>8.907182455062866</v>
+      </c>
+      <c r="G261" t="n">
+        <v>561.34473782537</v>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[1]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[1]) + np.max(np.abs(y)- 0.5,0)[1]*np.max(np.abs(y)- 0.5,0)[1]</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C262" t="n">
+        <v>2</v>
+      </c>
+      <c r="D262" t="n">
+        <v>2</v>
+      </c>
+      <c r="E262" t="n">
+        <v>0.0002519141708035022</v>
+      </c>
+      <c r="F262" t="n">
+        <v>8.495457887649536</v>
+      </c>
+      <c r="G262" t="n">
+        <v>588.5497952110225</v>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[1]) + np.max(np.abs(y)- 0.5,0)[1]*np.max(np.abs(y)- 0.5,0)[1]</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C263" t="n">
+        <v>1</v>
+      </c>
+      <c r="D263" t="n">
+        <v>1</v>
+      </c>
+      <c r="E263" t="n">
+        <v>0.0002929260081145912</v>
+      </c>
+      <c r="F263" t="n">
+        <v>6.327000617980957</v>
+      </c>
+      <c r="G263" t="n">
+        <v>790.2638709707566</v>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[1]) + np.max(np.abs(y)- 0.5,0)[1]*np.max(np.abs(y)- 0.5,0)[1]</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C264" t="n">
+        <v>1</v>
+      </c>
+      <c r="D264" t="n">
+        <v>1</v>
+      </c>
+      <c r="E264" t="n">
+        <v>0.000108376050775405</v>
+      </c>
+      <c r="F264" t="n">
+        <v>21.40224361419678</v>
+      </c>
+      <c r="G264" t="n">
+        <v>934.4814665474313</v>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>sqrt(np.max(np.abs(x) - 0.5,0)[0]) * np.sqrt(np.max(np.abs(x) - 0.5,0)[1]) + np.max(np.abs(y)- 0.5,0)[1]*np.max(np.abs(y)- 0.5,0)[1]</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>20000</v>
+      </c>
+      <c r="C265" t="n">
+        <v>1</v>
+      </c>
+      <c r="D265" t="n">
+        <v>1</v>
+      </c>
+      <c r="E265" t="n">
+        <v>0.01318632531911135</v>
+      </c>
+      <c r="F265" t="n">
+        <v>18.66489362716675</v>
+      </c>
+      <c r="G265" t="n">
+        <v>1071.530349944776</v>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>sqrt(torch.pow(torch.max(torch.abs(x) -  0.25,0).values,2) + torch.pow(torch.max(torch.abs(y) - 0.125,0).values,2))</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C266" t="n">
+        <v>1</v>
+      </c>
+      <c r="D266" t="n">
+        <v>1</v>
+      </c>
+      <c r="E266" t="n">
+        <v>7.335258851526305e-05</v>
+      </c>
+      <c r="F266" t="n">
+        <v>9.496311902999878</v>
+      </c>
+      <c r="G266" t="n">
+        <v>526.5201955319626</v>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>sqrt(torch.pow(torch.max(torch.abs(x) -  0.25,0).values,2) + torch.pow(torch.max(torch.abs(y) - 5.0,0).values,2))</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C267" t="n">
+        <v>1</v>
+      </c>
+      <c r="D267" t="n">
+        <v>1</v>
+      </c>
+      <c r="E267" t="n">
+        <v>0.0001131818280555308</v>
+      </c>
+      <c r="F267" t="n">
+        <v>9.584834814071655</v>
+      </c>
+      <c r="G267" t="n">
+        <v>521.6573991092071</v>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C268" t="n">
+        <v>1</v>
+      </c>
+      <c r="D268" t="n">
+        <v>1</v>
+      </c>
+      <c r="E268" t="n">
+        <v>2.21867120042518e-33</v>
+      </c>
+      <c r="F268" t="n">
+        <v>6.091338872909546</v>
+      </c>
+      <c r="G268" t="n">
+        <v>820.8376030821177</v>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C269" t="n">
+        <v>1</v>
+      </c>
+      <c r="D269" t="n">
+        <v>1</v>
+      </c>
+      <c r="E269" t="n">
+        <v>2.21867120042518e-33</v>
+      </c>
+      <c r="F269" t="n">
+        <v>4.638040065765381</v>
+      </c>
+      <c r="G269" t="n">
+        <v>1078.041571246084</v>
+      </c>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C270" t="n">
+        <v>1</v>
+      </c>
+      <c r="D270" t="n">
+        <v>1</v>
+      </c>
+      <c r="E270" t="n">
+        <v>2.21867120042518e-33</v>
+      </c>
+      <c r="F270" t="n">
+        <v>4.561209440231323</v>
+      </c>
+      <c r="G270" t="n">
+        <v>1096.200484875438</v>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C271" t="n">
+        <v>1</v>
+      </c>
+      <c r="D271" t="n">
+        <v>1</v>
+      </c>
+      <c r="E271" t="n">
+        <v>2.21867120042518e-33</v>
+      </c>
+      <c r="F271" t="n">
+        <v>5.78566312789917</v>
+      </c>
+      <c r="G271" t="n">
+        <v>864.2051722454066</v>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C272" t="n">
+        <v>1</v>
+      </c>
+      <c r="D272" t="n">
+        <v>1</v>
+      </c>
+      <c r="E272" t="n">
+        <v>2.21867120042518e-33</v>
+      </c>
+      <c r="F272" t="n">
+        <v>5.035567998886108</v>
+      </c>
+      <c r="G272" t="n">
+        <v>992.9366460955396</v>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C273" t="n">
+        <v>1</v>
+      </c>
+      <c r="D273" t="n">
+        <v>1</v>
+      </c>
+      <c r="E273" t="n">
+        <v>1.578964293003082e-05</v>
+      </c>
+      <c r="F273" t="n">
+        <v>5.136069774627686</v>
+      </c>
+      <c r="G273" t="n">
+        <v>973.5070237363453</v>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C274" t="n">
+        <v>1</v>
+      </c>
+      <c r="D274" t="n">
+        <v>1</v>
+      </c>
+      <c r="E274" t="n">
+        <v>0.006626044400036335</v>
+      </c>
+      <c r="F274" t="n">
+        <v>10.45488929748535</v>
+      </c>
+      <c r="G274" t="n">
+        <v>478.2451404055152</v>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C275" t="n">
+        <v>1</v>
+      </c>
+      <c r="D275" t="n">
+        <v>1</v>
+      </c>
+      <c r="E275" t="n">
+        <v>0.006626044400036335</v>
+      </c>
+      <c r="F275" t="n">
+        <v>9.139702558517456</v>
+      </c>
+      <c r="G275" t="n">
+        <v>547.0637548637081</v>
+      </c>
+      <c r="H275" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I275" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C276" t="n">
+        <v>1</v>
+      </c>
+      <c r="D276" t="n">
+        <v>1</v>
+      </c>
+      <c r="E276" t="n">
+        <v>0.003731169039383531</v>
+      </c>
+      <c r="F276" t="n">
+        <v>10.32171487808228</v>
+      </c>
+      <c r="G276" t="n">
+        <v>484.4156285131735</v>
+      </c>
+      <c r="H276" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I276" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>50000</v>
+      </c>
+      <c r="C277" t="n">
+        <v>1</v>
+      </c>
+      <c r="D277" t="n">
+        <v>1</v>
+      </c>
+      <c r="E277" t="n">
+        <v>0.003731165081262589</v>
+      </c>
+      <c r="F277" t="n">
+        <v>90.73556327819824</v>
+      </c>
+      <c r="G277" t="n">
+        <v>551.0518499422144</v>
+      </c>
+      <c r="H277" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I277" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C278" t="n">
+        <v>1</v>
+      </c>
+      <c r="D278" t="n">
+        <v>1</v>
+      </c>
+      <c r="E278" t="n">
+        <v>0.0007909532287158072</v>
+      </c>
+      <c r="F278" t="n">
+        <v>9.168042898178101</v>
+      </c>
+      <c r="G278" t="n">
+        <v>545.3726662855836</v>
+      </c>
+      <c r="H278" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I278" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C279" t="n">
+        <v>1</v>
+      </c>
+      <c r="D279" t="n">
+        <v>1</v>
+      </c>
+      <c r="E279" t="n">
+        <v>0.2579901218414307</v>
+      </c>
+      <c r="F279" t="n">
+        <v>9.818579435348511</v>
+      </c>
+      <c r="G279" t="n">
+        <v>509.2386360901835</v>
+      </c>
+      <c r="H279" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I279" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C280" t="n">
+        <v>1</v>
+      </c>
+      <c r="D280" t="n">
+        <v>1</v>
+      </c>
+      <c r="E280" t="n">
+        <v>0.2579901218414307</v>
+      </c>
+      <c r="F280" t="n">
+        <v>9.245616436004639</v>
+      </c>
+      <c r="G280" t="n">
+        <v>540.7968235118219</v>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C281" t="n">
+        <v>1</v>
+      </c>
+      <c r="D281" t="n">
+        <v>1</v>
+      </c>
+      <c r="E281" t="n">
+        <v>0.2579901218414307</v>
+      </c>
+      <c r="F281" t="n">
+        <v>9.440650224685669</v>
+      </c>
+      <c r="G281" t="n">
+        <v>529.6245365521396</v>
+      </c>
+      <c r="H281" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I281" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C282" t="n">
+        <v>1</v>
+      </c>
+      <c r="D282" t="n">
+        <v>1</v>
+      </c>
+      <c r="E282" t="n">
+        <v>0.0001173982964246534</v>
+      </c>
+      <c r="F282" t="n">
+        <v>11.37826132774353</v>
+      </c>
+      <c r="G282" t="n">
+        <v>439.4344492517971</v>
+      </c>
+      <c r="H282" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I282" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C283" t="n">
+        <v>1</v>
+      </c>
+      <c r="D283" t="n">
+        <v>1</v>
+      </c>
+      <c r="E283" t="n">
+        <v>0.0001173982964246534</v>
+      </c>
+      <c r="F283" t="n">
+        <v>9.879730939865112</v>
+      </c>
+      <c r="G283" t="n">
+        <v>506.0866566542616</v>
+      </c>
+      <c r="H283" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I283" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>50</v>
+      </c>
+      <c r="C284" t="n">
+        <v>1</v>
+      </c>
+      <c r="D284" t="n">
+        <v>1</v>
+      </c>
+      <c r="E284" t="n">
+        <v>0.492417186498642</v>
+      </c>
+      <c r="F284" t="n">
+        <v>0.6623921394348145</v>
+      </c>
+      <c r="G284" t="n">
+        <v>75.48398754046578</v>
+      </c>
+      <c r="H284" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I284" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C285" t="n">
+        <v>1</v>
+      </c>
+      <c r="D285" t="n">
+        <v>1</v>
+      </c>
+      <c r="E285" t="n">
+        <v>0.0001173982964246534</v>
+      </c>
+      <c r="F285" t="n">
+        <v>8.946409225463867</v>
+      </c>
+      <c r="G285" t="n">
+        <v>558.8834440714679</v>
+      </c>
+      <c r="H285" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I285" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.5</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C286" t="n">
+        <v>1</v>
+      </c>
+      <c r="D286" t="n">
+        <v>1</v>
+      </c>
+      <c r="E286" t="n">
+        <v>0.0001173982964246534</v>
+      </c>
+      <c r="F286" t="n">
+        <v>10.27708196640015</v>
+      </c>
+      <c r="G286" t="n">
+        <v>486.5194241270996</v>
+      </c>
+      <c r="H286" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I286" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C287" t="n">
+        <v>1</v>
+      </c>
+      <c r="D287" t="n">
+        <v>1</v>
+      </c>
+      <c r="E287" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F287" t="n">
+        <v>4.598223686218262</v>
+      </c>
+      <c r="G287" t="n">
+        <v>1087.376417764524</v>
+      </c>
+      <c r="H287" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C288" t="n">
+        <v>1</v>
+      </c>
+      <c r="D288" t="n">
+        <v>1</v>
+      </c>
+      <c r="E288" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F288" t="n">
+        <v>4.284999370574951</v>
+      </c>
+      <c r="G288" t="n">
+        <v>1166.86131492456</v>
+      </c>
+      <c r="H288" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I288" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C289" t="n">
+        <v>1</v>
+      </c>
+      <c r="D289" t="n">
+        <v>1</v>
+      </c>
+      <c r="E289" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F289" t="n">
+        <v>4.591999530792236</v>
+      </c>
+      <c r="G289" t="n">
+        <v>1088.850285474087</v>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C290" t="n">
+        <v>1</v>
+      </c>
+      <c r="D290" t="n">
+        <v>1</v>
+      </c>
+      <c r="E290" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F290" t="n">
+        <v>4.573186159133911</v>
+      </c>
+      <c r="G290" t="n">
+        <v>1093.329645025192</v>
+      </c>
+      <c r="H290" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I290" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C291" t="n">
+        <v>1</v>
+      </c>
+      <c r="D291" t="n">
+        <v>1</v>
+      </c>
+      <c r="E291" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F291" t="n">
+        <v>4.280056238174438</v>
+      </c>
+      <c r="G291" t="n">
+        <v>1168.208949079753</v>
+      </c>
+      <c r="H291" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I291" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C292" t="n">
+        <v>1</v>
+      </c>
+      <c r="D292" t="n">
+        <v>1</v>
+      </c>
+      <c r="E292" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F292" t="n">
+        <v>4.737054347991943</v>
+      </c>
+      <c r="G292" t="n">
+        <v>1055.508261609775</v>
+      </c>
+      <c r="H292" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I292" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C293" t="n">
+        <v>1</v>
+      </c>
+      <c r="D293" t="n">
+        <v>1</v>
+      </c>
+      <c r="E293" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F293" t="n">
+        <v>4.641098260879517</v>
+      </c>
+      <c r="G293" t="n">
+        <v>1077.331208896333</v>
+      </c>
+      <c r="H293" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I293" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C294" t="n">
+        <v>1</v>
+      </c>
+      <c r="D294" t="n">
+        <v>1</v>
+      </c>
+      <c r="E294" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F294" t="n">
+        <v>4.576636552810669</v>
+      </c>
+      <c r="G294" t="n">
+        <v>1092.505367709247</v>
+      </c>
+      <c r="H294" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I294" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C295" t="n">
+        <v>1</v>
+      </c>
+      <c r="D295" t="n">
+        <v>1</v>
+      </c>
+      <c r="E295" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F295" t="n">
+        <v>4.659013032913208</v>
+      </c>
+      <c r="G295" t="n">
+        <v>1073.18866993458</v>
+      </c>
+      <c r="H295" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I295" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C296" t="n">
+        <v>1</v>
+      </c>
+      <c r="D296" t="n">
+        <v>1</v>
+      </c>
+      <c r="E296" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F296" t="n">
+        <v>4.729764223098755</v>
+      </c>
+      <c r="G296" t="n">
+        <v>1057.135147579132</v>
+      </c>
+      <c r="H296" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I296" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C297" t="n">
+        <v>1</v>
+      </c>
+      <c r="D297" t="n">
+        <v>1</v>
+      </c>
+      <c r="E297" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F297" t="n">
+        <v>4.397030591964722</v>
+      </c>
+      <c r="G297" t="n">
+        <v>1137.131046833553</v>
+      </c>
+      <c r="H297" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I297" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C298" t="n">
+        <v>1</v>
+      </c>
+      <c r="D298" t="n">
+        <v>1</v>
+      </c>
+      <c r="E298" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F298" t="n">
+        <v>4.980543851852417</v>
+      </c>
+      <c r="G298" t="n">
+        <v>1003.906430447419</v>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C299" t="n">
+        <v>1</v>
+      </c>
+      <c r="D299" t="n">
+        <v>1</v>
+      </c>
+      <c r="E299" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F299" t="n">
+        <v>4.712598085403442</v>
+      </c>
+      <c r="G299" t="n">
+        <v>1060.985874328376</v>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C300" t="n">
+        <v>1</v>
+      </c>
+      <c r="D300" t="n">
+        <v>1</v>
+      </c>
+      <c r="E300" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F300" t="n">
+        <v>4.700301885604858</v>
+      </c>
+      <c r="G300" t="n">
+        <v>1063.761460793188</v>
+      </c>
+      <c r="H300" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I300" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C301" t="n">
+        <v>1</v>
+      </c>
+      <c r="D301" t="n">
+        <v>1</v>
+      </c>
+      <c r="E301" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F301" t="n">
+        <v>4.748921871185303</v>
+      </c>
+      <c r="G301" t="n">
+        <v>1052.870553701493</v>
+      </c>
+      <c r="H301" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I301" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C302" t="n">
+        <v>1</v>
+      </c>
+      <c r="D302" t="n">
+        <v>1</v>
+      </c>
+      <c r="E302" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F302" t="n">
+        <v>4.70733118057251</v>
+      </c>
+      <c r="G302" t="n">
+        <v>1062.17298256714</v>
+      </c>
+      <c r="H302" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I302" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C303" t="n">
+        <v>1</v>
+      </c>
+      <c r="D303" t="n">
+        <v>1</v>
+      </c>
+      <c r="E303" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F303" t="n">
+        <v>4.739624738693237</v>
+      </c>
+      <c r="G303" t="n">
+        <v>1054.935838945458</v>
+      </c>
+      <c r="H303" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I303" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>sqrt(torch.pow(torch.max(torch.abs(x) -  0.25,0).values,2) + torch.pow(torch.max(torch.abs(y) - 5.0,0).values,2))</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>500</v>
+      </c>
+      <c r="C304" t="n">
+        <v>1</v>
+      </c>
+      <c r="D304" t="n">
+        <v>1</v>
+      </c>
+      <c r="E304" t="n">
+        <v>0.001905889133922756</v>
+      </c>
+      <c r="F304" t="n">
+        <v>1.426330804824829</v>
+      </c>
+      <c r="G304" t="n">
+        <v>350.5498151681623</v>
+      </c>
+      <c r="H304" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I304" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>sqrt(torch.pow(torch.max(torch.abs(x) -  0.25,0).values,2) + torch.pow(torch.max(torch.abs(y) - 5.0,0).values,2))</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>500</v>
+      </c>
+      <c r="C305" t="n">
+        <v>1</v>
+      </c>
+      <c r="D305" t="n">
+        <v>1</v>
+      </c>
+      <c r="E305" t="n">
+        <v>0.001905889133922756</v>
+      </c>
+      <c r="F305" t="n">
+        <v>1.421339511871338</v>
+      </c>
+      <c r="G305" t="n">
+        <v>351.780834785701</v>
+      </c>
+      <c r="H305" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I305" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C306" t="n">
+        <v>1</v>
+      </c>
+      <c r="D306" t="n">
+        <v>1</v>
+      </c>
+      <c r="E306" t="n">
+        <v>0.000104373917565681</v>
+      </c>
+      <c r="F306" t="n">
+        <v>5.276967525482178</v>
+      </c>
+      <c r="G306" t="n">
+        <v>947.5138847937349</v>
+      </c>
+      <c r="H306" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I306" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>sqrt(torch.pow(torch.max(torch.abs(x) -  0.25,0).values,2) + torch.pow(torch.max(torch.abs(y) - 5.0,0).values,2))</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>500</v>
+      </c>
+      <c r="C307" t="n">
+        <v>1</v>
+      </c>
+      <c r="D307" t="n">
+        <v>1</v>
+      </c>
+      <c r="E307" t="n">
+        <v>0.03747707605361938</v>
+      </c>
+      <c r="F307" t="n">
+        <v>1.050745487213135</v>
+      </c>
+      <c r="G307" t="n">
+        <v>475.8526266204932</v>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>sqrt(torch.pow(torch.max(torch.abs(x) -  0.25,0).values,2) + torch.pow(torch.max(torch.abs(y) - 5.0,0).values,2))</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C308" t="n">
+        <v>1</v>
+      </c>
+      <c r="D308" t="n">
+        <v>1</v>
+      </c>
+      <c r="E308" t="n">
+        <v>0.0002007223229156807</v>
+      </c>
+      <c r="F308" t="n">
+        <v>4.647198677062988</v>
+      </c>
+      <c r="G308" t="n">
+        <v>1075.916987297815</v>
+      </c>
+      <c r="H308" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I308" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C309" t="n">
+        <v>1</v>
+      </c>
+      <c r="D309" t="n">
+        <v>1</v>
+      </c>
+      <c r="E309" t="n">
+        <v>0.008036335930228233</v>
+      </c>
+      <c r="F309" t="n">
+        <v>4.051060676574707</v>
+      </c>
+      <c r="G309" t="n">
+        <v>1234.244658173733</v>
+      </c>
+      <c r="H309" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I309" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C310" t="n">
+        <v>1</v>
+      </c>
+      <c r="D310" t="n">
+        <v>1</v>
+      </c>
+      <c r="E310" t="n">
+        <v>0.008036335930228233</v>
+      </c>
+      <c r="F310" t="n">
+        <v>4.035287380218506</v>
+      </c>
+      <c r="G310" t="n">
+        <v>1239.06912417456</v>
+      </c>
+      <c r="H310" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I310" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>sqrt(torch.pow(torch.max(torch.abs(x) -  0.25,0).values,2) + torch.pow(torch.max(torch.abs(y) - 5.0,0).values,2))</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C311" t="n">
+        <v>1</v>
+      </c>
+      <c r="D311" t="n">
+        <v>1</v>
+      </c>
+      <c r="E311" t="n">
+        <v>0.04884292930364609</v>
+      </c>
+      <c r="F311" t="n">
+        <v>3.823054790496826</v>
+      </c>
+      <c r="G311" t="n">
+        <v>1307.85465393506</v>
+      </c>
+      <c r="H311" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I311" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C312" t="n">
+        <v>1</v>
+      </c>
+      <c r="D312" t="n">
+        <v>1</v>
+      </c>
+      <c r="E312" t="n">
+        <v>0.00860558170825243</v>
+      </c>
+      <c r="F312" t="n">
+        <v>4.067296743392944</v>
+      </c>
+      <c r="G312" t="n">
+        <v>1229.317730043221</v>
+      </c>
+      <c r="H312" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I312" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C313" t="n">
+        <v>1</v>
+      </c>
+      <c r="D313" t="n">
+        <v>1</v>
+      </c>
+      <c r="E313" t="n">
+        <v>0.008455374278128147</v>
+      </c>
+      <c r="F313" t="n">
+        <v>4.025999784469604</v>
+      </c>
+      <c r="G313" t="n">
+        <v>1241.927537921792</v>
+      </c>
+      <c r="H313" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I313" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C314" t="n">
+        <v>1</v>
+      </c>
+      <c r="D314" t="n">
+        <v>1</v>
+      </c>
+      <c r="E314" t="n">
+        <v>0.008455337025225163</v>
+      </c>
+      <c r="F314" t="n">
+        <v>4.047111749649048</v>
+      </c>
+      <c r="G314" t="n">
+        <v>1235.44895947921</v>
+      </c>
+      <c r="H314" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I314" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C315" t="n">
+        <v>1</v>
+      </c>
+      <c r="D315" t="n">
+        <v>1</v>
+      </c>
+      <c r="E315" t="n">
+        <v>0.0084574269130826</v>
+      </c>
+      <c r="F315" t="n">
+        <v>4.012049674987793</v>
+      </c>
+      <c r="G315" t="n">
+        <v>1246.245785831456</v>
+      </c>
+      <c r="H315" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I315" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C316" t="n">
+        <v>1</v>
+      </c>
+      <c r="D316" t="n">
+        <v>1</v>
+      </c>
+      <c r="E316" t="n">
+        <v>0.008455361239612103</v>
+      </c>
+      <c r="F316" t="n">
+        <v>4.044855117797852</v>
+      </c>
+      <c r="G316" t="n">
+        <v>1236.13821864704</v>
+      </c>
+      <c r="H316" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I316" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C317" t="n">
+        <v>1</v>
+      </c>
+      <c r="D317" t="n">
+        <v>1</v>
+      </c>
+      <c r="E317" t="n">
+        <v>0.003187325783073902</v>
+      </c>
+      <c r="F317" t="n">
+        <v>5.679396152496338</v>
+      </c>
+      <c r="G317" t="n">
+        <v>880.3752838763124</v>
+      </c>
+      <c r="H317" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I317" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C318" t="n">
+        <v>1</v>
+      </c>
+      <c r="D318" t="n">
+        <v>1</v>
+      </c>
+      <c r="E318" t="n">
+        <v>5.136120762472274e-06</v>
+      </c>
+      <c r="F318" t="n">
+        <v>4.651704549789429</v>
+      </c>
+      <c r="G318" t="n">
+        <v>1074.87480051293</v>
+      </c>
+      <c r="H318" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I318" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.1</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>100</v>
+      </c>
+      <c r="C319" t="n">
+        <v>1</v>
+      </c>
+      <c r="D319" t="n">
+        <v>1</v>
+      </c>
+      <c r="E319" t="n">
+        <v>1.022018295770977e-06</v>
+      </c>
+      <c r="F319" t="n">
+        <v>1.070050954818726</v>
+      </c>
+      <c r="G319" t="n">
+        <v>93.4534935459599</v>
+      </c>
+      <c r="H319" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I319" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.3</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C320" t="n">
+        <v>1</v>
+      </c>
+      <c r="D320" t="n">
+        <v>1</v>
+      </c>
+      <c r="E320" t="n">
+        <v>4.322128916101065e-06</v>
+      </c>
+      <c r="F320" t="n">
+        <v>4.097027778625488</v>
+      </c>
+      <c r="G320" t="n">
+        <v>1220.396899939363</v>
+      </c>
+      <c r="H320" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I320" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.3</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C321" t="n">
+        <v>1</v>
+      </c>
+      <c r="D321" t="n">
+        <v>1</v>
+      </c>
+      <c r="E321" t="n">
+        <v>1.600677251190064e-06</v>
+      </c>
+      <c r="F321" t="n">
+        <v>4.119686841964722</v>
+      </c>
+      <c r="G321" t="n">
+        <v>1213.68448423508</v>
+      </c>
+      <c r="H321" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I321" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.3</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C322" t="n">
+        <v>1</v>
+      </c>
+      <c r="D322" t="n">
+        <v>1</v>
+      </c>
+      <c r="E322" t="n">
+        <v>6.193059842729554e-09</v>
+      </c>
+      <c r="F322" t="n">
+        <v>4.186306476593018</v>
+      </c>
+      <c r="G322" t="n">
+        <v>1194.370270776066</v>
+      </c>
+      <c r="H322" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I322" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.3</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C323" t="n">
+        <v>1</v>
+      </c>
+      <c r="D323" t="n">
+        <v>1</v>
+      </c>
+      <c r="E323" t="n">
+        <v>7.010657299133527e-08</v>
+      </c>
+      <c r="F323" t="n">
+        <v>4.185302972793579</v>
+      </c>
+      <c r="G323" t="n">
+        <v>1194.656643139656</v>
+      </c>
+      <c r="H323" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I323" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C324" t="n">
+        <v>1</v>
+      </c>
+      <c r="D324" t="n">
+        <v>1</v>
+      </c>
+      <c r="E324" t="n">
+        <v>3.020556027522048e-09</v>
+      </c>
+      <c r="F324" t="n">
+        <v>151.4999315738678</v>
+      </c>
+      <c r="G324" t="n">
+        <v>33.00331523623242</v>
+      </c>
+      <c r="H324" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I324" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C325" t="n">
+        <v>1</v>
+      </c>
+      <c r="D325" t="n">
+        <v>1</v>
+      </c>
+      <c r="E325" t="n">
+        <v>5.917643264297112e-09</v>
+      </c>
+      <c r="F325" t="n">
+        <v>150.2054860591888</v>
+      </c>
+      <c r="G325" t="n">
+        <v>33.28773223389283</v>
+      </c>
+      <c r="H325" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I325" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C326" t="n">
+        <v>1</v>
+      </c>
+      <c r="D326" t="n">
+        <v>1</v>
+      </c>
+      <c r="E326" t="n">
+        <v>4.540357281257457e-07</v>
+      </c>
+      <c r="F326" t="n">
+        <v>149.0031487941742</v>
+      </c>
+      <c r="G326" t="n">
+        <v>33.55633783891883</v>
+      </c>
+      <c r="H326" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I326" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C327" t="n">
+        <v>1</v>
+      </c>
+      <c r="D327" t="n">
+        <v>1</v>
+      </c>
+      <c r="E327" t="n">
+        <v>2.341034360142658e-06</v>
+      </c>
+      <c r="F327" t="n">
+        <v>4.053073883056641</v>
+      </c>
+      <c r="G327" t="n">
+        <v>1233.631595244751</v>
+      </c>
+      <c r="H327" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I327" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C328" t="n">
+        <v>1</v>
+      </c>
+      <c r="D328" t="n">
+        <v>1</v>
+      </c>
+      <c r="E328" t="n">
+        <v>1.674067817702962e-07</v>
+      </c>
+      <c r="F328" t="n">
+        <v>4.286120414733887</v>
+      </c>
+      <c r="G328" t="n">
+        <v>1166.556119798243</v>
+      </c>
+      <c r="H328" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I328" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C329" t="n">
+        <v>5</v>
+      </c>
+      <c r="D329" t="n">
+        <v>5</v>
+      </c>
+      <c r="E329" t="n">
+        <v>2.350384420424234e-05</v>
+      </c>
+      <c r="F329" t="n">
+        <v>9.388856410980225</v>
+      </c>
+      <c r="G329" t="n">
+        <v>532.5462208744106</v>
+      </c>
+      <c r="H329" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I329" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C330" t="n">
+        <v>1</v>
+      </c>
+      <c r="D330" t="n">
+        <v>1</v>
+      </c>
+      <c r="E330" t="n">
+        <v>0.001604624325409532</v>
+      </c>
+      <c r="F330" t="n">
+        <v>3.964118242263794</v>
+      </c>
+      <c r="G330" t="n">
+        <v>1261.314545739848</v>
+      </c>
+      <c r="H330" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I330" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C331" t="n">
+        <v>8</v>
+      </c>
+      <c r="D331" t="n">
+        <v>8</v>
+      </c>
+      <c r="E331" t="n">
+        <v>0.001604740391485393</v>
+      </c>
+      <c r="F331" t="n">
+        <v>13.52890658378601</v>
+      </c>
+      <c r="G331" t="n">
+        <v>369.579017271976</v>
+      </c>
+      <c r="H331" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I331" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C332" t="n">
+        <v>2</v>
+      </c>
+      <c r="D332" t="n">
+        <v>2</v>
+      </c>
+      <c r="E332" t="n">
+        <v>0.001604657038114965</v>
+      </c>
+      <c r="F332" t="n">
+        <v>5.386520862579346</v>
+      </c>
+      <c r="G332" t="n">
+        <v>928.2429470821246</v>
+      </c>
+      <c r="H332" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I332" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C333" t="n">
+        <v>1</v>
+      </c>
+      <c r="D333" t="n">
+        <v>1</v>
+      </c>
+      <c r="E333" t="n">
+        <v>1.55724846990779e-05</v>
+      </c>
+      <c r="F333" t="n">
+        <v>9.792124032974243</v>
+      </c>
+      <c r="G333" t="n">
+        <v>510.6144471988789</v>
+      </c>
+      <c r="H333" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I333" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C334" t="n">
+        <v>16</v>
+      </c>
+      <c r="D334" t="n">
+        <v>16</v>
+      </c>
+      <c r="E334" t="n">
+        <v>2.90024877358519e-06</v>
+      </c>
+      <c r="F334" t="n">
+        <v>45.12263822555542</v>
+      </c>
+      <c r="G334" t="n">
+        <v>110.8091236821394</v>
+      </c>
+      <c r="H334" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I334" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B335" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C335" t="n">
+        <v>2</v>
+      </c>
+      <c r="D335" t="n">
+        <v>2</v>
+      </c>
+      <c r="E335" t="n">
+        <v>2.714868060138542e-05</v>
+      </c>
+      <c r="F335" t="n">
+        <v>6.450606107711792</v>
+      </c>
+      <c r="G335" t="n">
+        <v>775.1209601873579</v>
+      </c>
+      <c r="H335" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I335" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B336" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C336" t="n">
+        <v>2</v>
+      </c>
+      <c r="D336" t="n">
+        <v>2</v>
+      </c>
+      <c r="E336" t="n">
+        <v>0.0002564094320405275</v>
+      </c>
+      <c r="F336" t="n">
+        <v>5.702149152755737</v>
+      </c>
+      <c r="G336" t="n">
+        <v>876.8623664611786</v>
+      </c>
+      <c r="H336" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I336" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C337" t="n">
+        <v>2</v>
+      </c>
+      <c r="D337" t="n">
+        <v>2</v>
+      </c>
+      <c r="E337" t="n">
+        <v>0.0002424973645247519</v>
+      </c>
+      <c r="F337" t="n">
+        <v>5.555581331253052</v>
+      </c>
+      <c r="G337" t="n">
+        <v>899.995824356379</v>
+      </c>
+      <c r="H337" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I337" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B338" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C338" t="n">
+        <v>1</v>
+      </c>
+      <c r="D338" t="n">
+        <v>1</v>
+      </c>
+      <c r="E338" t="n">
+        <v>0.0002564086462371051</v>
+      </c>
+      <c r="F338" t="n">
+        <v>4.160150051116943</v>
+      </c>
+      <c r="G338" t="n">
+        <v>1201.879725145387</v>
+      </c>
+      <c r="H338" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I338" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B339" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C339" t="n">
+        <v>4</v>
+      </c>
+      <c r="D339" t="n">
+        <v>4</v>
+      </c>
+      <c r="E339" t="n">
+        <v>0.0002564086462371051</v>
+      </c>
+      <c r="F339" t="n">
+        <v>7.535049438476562</v>
+      </c>
+      <c r="G339" t="n">
+        <v>663.5656528633077</v>
+      </c>
+      <c r="H339" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I339" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B340" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C340" t="n">
+        <v>8</v>
+      </c>
+      <c r="D340" t="n">
+        <v>8</v>
+      </c>
+      <c r="E340" t="n">
+        <v>0.0002564084134064615</v>
+      </c>
+      <c r="F340" t="n">
+        <v>13.20914077758789</v>
+      </c>
+      <c r="G340" t="n">
+        <v>378.5257560797263</v>
+      </c>
+      <c r="H340" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I340" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B341" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C341" t="n">
+        <v>16</v>
+      </c>
+      <c r="D341" t="n">
+        <v>16</v>
+      </c>
+      <c r="E341" t="n">
+        <v>7.753130194032565e-05</v>
+      </c>
+      <c r="F341" t="n">
+        <v>25.30251049995422</v>
+      </c>
+      <c r="G341" t="n">
+        <v>197.6088499206055</v>
+      </c>
+      <c r="H341" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I341" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B342" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C342" t="n">
+        <v>16</v>
+      </c>
+      <c r="D342" t="n">
+        <v>16</v>
+      </c>
+      <c r="E342" t="n">
+        <v>0.0002564846945460886</v>
+      </c>
+      <c r="F342" t="n">
+        <v>25.49650406837463</v>
+      </c>
+      <c r="G342" t="n">
+        <v>196.1053165010925</v>
+      </c>
+      <c r="H342" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I342" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B343" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C343" t="n">
+        <v>1</v>
+      </c>
+      <c r="D343" t="n">
+        <v>1</v>
+      </c>
+      <c r="E343" t="n">
+        <v>0.0002571482618805021</v>
+      </c>
+      <c r="F343" t="n">
+        <v>4.31634783744812</v>
+      </c>
+      <c r="G343" t="n">
+        <v>1158.386716802709</v>
+      </c>
+      <c r="H343" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I343" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B344" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C344" t="n">
+        <v>1</v>
+      </c>
+      <c r="D344" t="n">
+        <v>1</v>
+      </c>
+      <c r="E344" t="n">
+        <v>0.0001740958541631699</v>
+      </c>
+      <c r="F344" t="n">
+        <v>4.199733972549438</v>
+      </c>
+      <c r="G344" t="n">
+        <v>1190.551599858779</v>
+      </c>
+      <c r="H344" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I344" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B345" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C345" t="n">
+        <v>64</v>
+      </c>
+      <c r="D345" t="n">
+        <v>64</v>
+      </c>
+      <c r="E345" t="n">
+        <v>0.0002564426977187395</v>
+      </c>
+      <c r="F345" t="n">
+        <v>84.8508939743042</v>
+      </c>
+      <c r="G345" t="n">
+        <v>58.92689830132107</v>
+      </c>
+      <c r="H345" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I345" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B346" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C346" t="n">
+        <v>64</v>
+      </c>
+      <c r="D346" t="n">
+        <v>64</v>
+      </c>
+      <c r="E346" t="n">
+        <v>0.0002025492285611108</v>
+      </c>
+      <c r="F346" t="n">
+        <v>84.98574066162109</v>
+      </c>
+      <c r="G346" t="n">
+        <v>58.83339912171833</v>
+      </c>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B347" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C347" t="n">
+        <v>64</v>
+      </c>
+      <c r="D347" t="n">
+        <v>64</v>
+      </c>
+      <c r="E347" t="n">
+        <v>0.0002564183378126472</v>
+      </c>
+      <c r="F347" t="n">
+        <v>86.34745407104492</v>
+      </c>
+      <c r="G347" t="n">
+        <v>57.90558683856622</v>
+      </c>
+      <c r="H347" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I347" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B348" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C348" t="n">
+        <v>64</v>
+      </c>
+      <c r="D348" t="n">
+        <v>64</v>
+      </c>
+      <c r="E348" t="n">
+        <v>0.1468464136123657</v>
+      </c>
+      <c r="F348" t="n">
+        <v>86.42637228965759</v>
+      </c>
+      <c r="G348" t="n">
+        <v>57.85271170751588</v>
+      </c>
+      <c r="H348" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I348" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B349" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C349" t="n">
+        <v>64</v>
+      </c>
+      <c r="D349" t="n">
+        <v>64</v>
+      </c>
+      <c r="E349" t="n">
+        <v>0.0003028346982318908</v>
+      </c>
+      <c r="F349" t="n">
+        <v>87.07661509513855</v>
+      </c>
+      <c r="G349" t="n">
+        <v>57.42069779052709</v>
+      </c>
+      <c r="H349" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I349" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B350" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C350" t="n">
+        <v>64</v>
+      </c>
+      <c r="D350" t="n">
+        <v>64</v>
+      </c>
+      <c r="E350" t="n">
+        <v>0.009801116771996021</v>
+      </c>
+      <c r="F350" t="n">
+        <v>87.30866169929504</v>
+      </c>
+      <c r="G350" t="n">
+        <v>57.26808661001812</v>
+      </c>
+      <c r="H350" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I350" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B351" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C351" t="n">
+        <v>64</v>
+      </c>
+      <c r="D351" t="n">
+        <v>64</v>
+      </c>
+      <c r="E351" t="n">
+        <v>6.68601614961517e-06</v>
+      </c>
+      <c r="F351" t="n">
+        <v>86.51183772087097</v>
+      </c>
+      <c r="G351" t="n">
+        <v>57.79555875500435</v>
+      </c>
+      <c r="H351" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I351" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B352" t="n">
+        <v>550</v>
+      </c>
+      <c r="C352" t="n">
+        <v>64</v>
+      </c>
+      <c r="D352" t="n">
+        <v>64</v>
+      </c>
+      <c r="E352" t="n">
+        <v>0.6354044079780579</v>
+      </c>
+      <c r="F352" t="n">
+        <v>9.75135350227356</v>
+      </c>
+      <c r="G352" t="n">
+        <v>56.40242658332156</v>
+      </c>
+      <c r="H352" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I352" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B353" t="n">
+        <v>560</v>
+      </c>
+      <c r="C353" t="n">
+        <v>1</v>
+      </c>
+      <c r="D353" t="n">
+        <v>1</v>
+      </c>
+      <c r="E353" t="n">
+        <v>0.0001319747098023072</v>
+      </c>
+      <c r="F353" t="n">
+        <v>1.288227319717407</v>
+      </c>
+      <c r="G353" t="n">
+        <v>434.7058872519834</v>
+      </c>
+      <c r="H353" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I353" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B354" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C354" t="n">
+        <v>1</v>
+      </c>
+      <c r="D354" t="n">
+        <v>1</v>
+      </c>
+      <c r="E354" t="n">
+        <v>0.0001530168810859323</v>
+      </c>
+      <c r="F354" t="n">
+        <v>4.434500932693481</v>
+      </c>
+      <c r="G354" t="n">
+        <v>1127.522595189317</v>
+      </c>
+      <c r="H354" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I354" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B355" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C355" t="n">
+        <v>128</v>
+      </c>
+      <c r="D355" t="n">
+        <v>128</v>
+      </c>
+      <c r="E355" t="n">
+        <v>2.760958705039229e-05</v>
+      </c>
+      <c r="F355" t="n">
+        <v>161.3457019329071</v>
+      </c>
+      <c r="G355" t="n">
+        <v>30.989359741849</v>
+      </c>
+      <c r="H355" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I355" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B356" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C356" t="n">
+        <v>1</v>
+      </c>
+      <c r="D356" t="n">
+        <v>1</v>
+      </c>
+      <c r="E356" t="n">
+        <v>6.880718137836084e-05</v>
+      </c>
+      <c r="F356" t="n">
+        <v>4.611052513122559</v>
+      </c>
+      <c r="G356" t="n">
+        <v>1084.35112932905</v>
+      </c>
+      <c r="H356" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I356" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B357" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C357" t="n">
+        <v>1</v>
+      </c>
+      <c r="D357" t="n">
+        <v>1</v>
+      </c>
+      <c r="E357" t="n">
+        <v>0.0003578454197850078</v>
+      </c>
+      <c r="F357" t="n">
+        <v>6.038472414016724</v>
+      </c>
+      <c r="G357" t="n">
+        <v>828.0239863965953</v>
+      </c>
+      <c r="H357" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I357" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B358" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C358" t="n">
+        <v>16</v>
+      </c>
+      <c r="D358" t="n">
+        <v>16</v>
+      </c>
+      <c r="E358" t="n">
+        <v>4.308887127990602e-06</v>
+      </c>
+      <c r="F358" t="n">
+        <v>25.61848211288452</v>
+      </c>
+      <c r="G358" t="n">
+        <v>195.1715943968947</v>
+      </c>
+      <c r="H358" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I358" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.4</t>
+        </is>
+      </c>
+      <c r="B359" t="n">
+        <v>50000</v>
+      </c>
+      <c r="C359" t="n">
+        <v>16</v>
+      </c>
+      <c r="D359" t="n">
+        <v>16</v>
+      </c>
+      <c r="E359" t="n">
+        <v>0.01013930793851614</v>
+      </c>
+      <c r="F359" t="n">
+        <v>845.8728001117706</v>
+      </c>
+      <c r="G359" t="n">
+        <v>59.11054238106862</v>
+      </c>
+      <c r="H359" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I359" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B360" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C360" t="n">
+        <v>1</v>
+      </c>
+      <c r="D360" t="n">
+        <v>1</v>
+      </c>
+      <c r="E360" t="n">
+        <v>3.753086708600806e-13</v>
+      </c>
+      <c r="F360" t="n">
+        <v>4.641128540039062</v>
+      </c>
+      <c r="G360" t="n">
+        <v>1077.324180286098</v>
+      </c>
+      <c r="H360" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I360" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 1.0</t>
+        </is>
+      </c>
+      <c r="B361" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C361" t="n">
+        <v>1</v>
+      </c>
+      <c r="D361" t="n">
+        <v>1</v>
+      </c>
+      <c r="E361" t="n">
+        <v>7.313714013434947e-05</v>
+      </c>
+      <c r="F361" t="n">
+        <v>3.883069753646851</v>
+      </c>
+      <c r="G361" t="n">
+        <v>1287.641046186246</v>
+      </c>
+      <c r="H361" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I361" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B362" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C362" t="n">
+        <v>1</v>
+      </c>
+      <c r="D362" t="n">
+        <v>1</v>
+      </c>
+      <c r="E362" t="n">
+        <v>0.0001358724402962252</v>
+      </c>
+      <c r="F362" t="n">
+        <v>3.572728395462036</v>
+      </c>
+      <c r="G362" t="n">
+        <v>1399.490654355601</v>
+      </c>
+      <c r="H362" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I362" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B363" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C363" t="n">
+        <v>1</v>
+      </c>
+      <c r="D363" t="n">
+        <v>1</v>
+      </c>
+      <c r="E363" t="n">
+        <v>8.552065992262214e-05</v>
+      </c>
+      <c r="F363" t="n">
+        <v>4.310048341751099</v>
+      </c>
+      <c r="G363" t="n">
+        <v>1160.079795756673</v>
+      </c>
+      <c r="H363" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I363" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B364" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C364" t="n">
+        <v>16</v>
+      </c>
+      <c r="D364" t="n">
+        <v>16</v>
+      </c>
+      <c r="E364" t="n">
+        <v>0.05017779394984245</v>
+      </c>
+      <c r="F364" t="n">
+        <v>22.79969453811646</v>
+      </c>
+      <c r="G364" t="n">
+        <v>219.301183690905</v>
+      </c>
+      <c r="H364" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I364" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B365" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C365" t="n">
+        <v>1</v>
+      </c>
+      <c r="D365" t="n">
+        <v>1</v>
+      </c>
+      <c r="E365" t="n">
+        <v>1.583953235240187e-08</v>
+      </c>
+      <c r="F365" t="n">
+        <v>8.678031444549561</v>
+      </c>
+      <c r="G365" t="n">
+        <v>576.1675366065153</v>
+      </c>
+      <c r="H365" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I365" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B366" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C366" t="n">
+        <v>1</v>
+      </c>
+      <c r="D366" t="n">
+        <v>1</v>
+      </c>
+      <c r="E366" t="n">
+        <v>3.728202102593059e-07</v>
+      </c>
+      <c r="F366" t="n">
+        <v>8.61081862449646</v>
+      </c>
+      <c r="G366" t="n">
+        <v>580.6648842626607</v>
+      </c>
+      <c r="H366" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I366" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B367" t="n">
+        <v>500</v>
+      </c>
+      <c r="C367" t="n">
+        <v>1</v>
+      </c>
+      <c r="D367" t="n">
+        <v>1</v>
+      </c>
+      <c r="E367" t="n">
+        <v>8.815665637484926e-07</v>
+      </c>
+      <c r="F367" t="n">
+        <v>1.766450881958008</v>
+      </c>
+      <c r="G367" t="n">
+        <v>283.0534407193814</v>
+      </c>
+      <c r="H367" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I367" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B368" t="n">
+        <v>500</v>
+      </c>
+      <c r="C368" t="n">
+        <v>1</v>
+      </c>
+      <c r="D368" t="n">
+        <v>1</v>
+      </c>
+      <c r="E368" t="n">
+        <v>9.32150145429655e-35</v>
+      </c>
+      <c r="F368" t="n">
+        <v>0.9530048370361328</v>
+      </c>
+      <c r="G368" t="n">
+        <v>524.6563087287276</v>
+      </c>
+      <c r="H368" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I368" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.2</t>
+        </is>
+      </c>
+      <c r="B369" t="n">
+        <v>500</v>
+      </c>
+      <c r="C369" t="n">
+        <v>16</v>
+      </c>
+      <c r="D369" t="n">
+        <v>16</v>
+      </c>
+      <c r="E369" t="n">
+        <v>3.389591483937693e-06</v>
+      </c>
+      <c r="F369" t="n">
+        <v>2.81590747833252</v>
+      </c>
+      <c r="G369" t="n">
+        <v>177.5626521280743</v>
+      </c>
+      <c r="H369" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I369" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B370" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C370" t="n">
+        <v>1</v>
+      </c>
+      <c r="D370" t="n">
+        <v>1</v>
+      </c>
+      <c r="E370" t="n">
+        <v>1.647402541493648e-06</v>
+      </c>
+      <c r="F370" t="n">
+        <v>4.100343704223633</v>
+      </c>
+      <c r="G370" t="n">
+        <v>1219.409971620101</v>
+      </c>
+      <c r="H370" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I370" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B371" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C371" t="n">
+        <v>1</v>
+      </c>
+      <c r="D371" t="n">
+        <v>1</v>
+      </c>
+      <c r="E371" t="n">
+        <v>1.021055140881799e-06</v>
+      </c>
+      <c r="F371" t="n">
+        <v>4.274586915969849</v>
+      </c>
+      <c r="G371" t="n">
+        <v>1169.703669217722</v>
+      </c>
+      <c r="H371" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I371" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B372" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C372" t="n">
+        <v>2</v>
+      </c>
+      <c r="D372" t="n">
+        <v>0</v>
+      </c>
+      <c r="E372" t="n">
+        <v>0</v>
+      </c>
+      <c r="F372" t="n">
+        <v>4.090194225311279</v>
+      </c>
+      <c r="G372" t="n">
+        <v>1222.435836679487</v>
+      </c>
+      <c r="H372" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I372" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B373" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C373" t="n">
+        <v>2</v>
+      </c>
+      <c r="D373" t="n">
+        <v>2</v>
+      </c>
+      <c r="E373" t="n">
+        <v>0.0002480322727933526</v>
+      </c>
+      <c r="F373" t="n">
+        <v>4.949307441711426</v>
+      </c>
+      <c r="G373" t="n">
+        <v>1010.242353881949</v>
+      </c>
+      <c r="H373" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I373" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B374" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C374" t="n">
+        <v>4</v>
+      </c>
+      <c r="D374" t="n">
+        <v>4</v>
+      </c>
+      <c r="E374" t="n">
+        <v>1.510899068080107e-07</v>
+      </c>
+      <c r="F374" t="n">
+        <v>8.229551792144775</v>
+      </c>
+      <c r="G374" t="n">
+        <v>607.5665025612417</v>
+      </c>
+      <c r="H374" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I374" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B375" t="n">
+        <v>1</v>
+      </c>
+      <c r="C375" t="n">
+        <v>4</v>
+      </c>
+      <c r="D375" t="n">
+        <v>4</v>
+      </c>
+      <c r="E375" t="n">
+        <v>0.3149298429489136</v>
+      </c>
+      <c r="F375" t="n">
+        <v>0.6160197257995605</v>
+      </c>
+      <c r="G375" t="n">
+        <v>1.623324640622593</v>
+      </c>
+      <c r="H375" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I375" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B376" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C376" t="n">
+        <v>4</v>
+      </c>
+      <c r="D376" t="n">
+        <v>4</v>
+      </c>
+      <c r="E376" t="n">
+        <v>0.003002032870426774</v>
+      </c>
+      <c r="F376" t="n">
+        <v>2.130999088287354</v>
+      </c>
+      <c r="G376" t="n">
+        <v>469.2634574535095</v>
+      </c>
+      <c r="H376" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I376" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B377" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C377" t="n">
+        <v>4</v>
+      </c>
+      <c r="D377" t="n">
+        <v>4</v>
+      </c>
+      <c r="E377" t="n">
+        <v>5.151434834260726e-14</v>
+      </c>
+      <c r="F377" t="n">
+        <v>2.132013559341431</v>
+      </c>
+      <c r="G377" t="n">
+        <v>469.0401689137922</v>
+      </c>
+      <c r="H377" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B378" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C378" t="n">
+        <v>1</v>
+      </c>
+      <c r="D378" t="n">
+        <v>1</v>
+      </c>
+      <c r="E378" t="n">
+        <v>1.546141077039646e-14</v>
+      </c>
+      <c r="F378" t="n">
+        <v>8.690387964248657</v>
+      </c>
+      <c r="G378" t="n">
+        <v>575.3483067234138</v>
+      </c>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B379" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C379" t="n">
+        <v>1</v>
+      </c>
+      <c r="D379" t="n">
+        <v>1</v>
+      </c>
+      <c r="E379" t="n">
+        <v>1.999274132913342e-07</v>
+      </c>
+      <c r="F379" t="n">
+        <v>8.950819730758667</v>
+      </c>
+      <c r="G379" t="n">
+        <v>558.6080549491977</v>
+      </c>
+      <c r="H379" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I379" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B380" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C380" t="n">
+        <v>1</v>
+      </c>
+      <c r="D380" t="n">
+        <v>1</v>
+      </c>
+      <c r="E380" t="n">
+        <v>0.0003619201888795942</v>
+      </c>
+      <c r="F380" t="n">
+        <v>9.499584197998047</v>
+      </c>
+      <c r="G380" t="n">
+        <v>526.3388266039798</v>
+      </c>
+      <c r="H380" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I380" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B381" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C381" t="n">
+        <v>1</v>
+      </c>
+      <c r="D381" t="n">
+        <v>1</v>
+      </c>
+      <c r="E381" t="n">
+        <v>0.0001180996478069574</v>
+      </c>
+      <c r="F381" t="n">
+        <v>8.928579807281494</v>
+      </c>
+      <c r="G381" t="n">
+        <v>559.9994744877978</v>
+      </c>
+      <c r="H381" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I381" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>sqrt(x**2 + y**2) - 0.25</t>
+        </is>
+      </c>
+      <c r="B382" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C382" t="n">
+        <v>32</v>
+      </c>
+      <c r="D382" t="n">
+        <v>32</v>
+      </c>
+      <c r="E382" t="n">
+        <v>0.001675377599895</v>
+      </c>
+      <c r="F382" t="n">
+        <v>4633.21964597702</v>
+      </c>
+      <c r="G382" t="n">
+        <v>1.079163169900968</v>
+      </c>
+      <c r="H382" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I382" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>